<commit_message>
modified:   mentor2_result.txt 	modified:   nodes_inf.xlsx 	modified:   mentor2_result.txt 	modified:   nodes_inf.xlsx
</commit_message>
<xml_diff>
--- a/nodes_inf.xlsx
+++ b/nodes_inf.xlsx
@@ -459,10 +459,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>221</v>
+        <v>518</v>
       </c>
       <c r="C2" t="n">
-        <v>688</v>
+        <v>59</v>
       </c>
       <c r="D2" t="n">
         <v>11</v>
@@ -473,10 +473,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>243</v>
+        <v>790</v>
       </c>
       <c r="C3" t="n">
-        <v>41</v>
+        <v>840</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -487,10 +487,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>782</v>
+        <v>96</v>
       </c>
       <c r="C4" t="n">
-        <v>531</v>
+        <v>433</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
@@ -501,10 +501,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>91</v>
+        <v>882</v>
       </c>
       <c r="C5" t="n">
-        <v>210</v>
+        <v>598</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
@@ -515,10 +515,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>885</v>
+        <v>95</v>
       </c>
       <c r="C6" t="n">
-        <v>204</v>
+        <v>742</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
@@ -529,10 +529,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>774</v>
+        <v>502</v>
       </c>
       <c r="C7" t="n">
-        <v>267</v>
+        <v>186</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
@@ -543,10 +543,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>58</v>
+        <v>492</v>
       </c>
       <c r="C8" t="n">
-        <v>438</v>
+        <v>645</v>
       </c>
       <c r="D8" t="n">
         <v>5</v>
@@ -557,10 +557,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>871</v>
+        <v>829</v>
       </c>
       <c r="C9" t="n">
-        <v>858</v>
+        <v>389</v>
       </c>
       <c r="D9" t="n">
         <v>51</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C10" t="n">
-        <v>526</v>
+        <v>168</v>
       </c>
       <c r="D10" t="n">
         <v>5</v>
@@ -585,10 +585,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>939</v>
+        <v>604</v>
       </c>
       <c r="C11" t="n">
-        <v>936</v>
+        <v>201</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -599,10 +599,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>53</v>
+        <v>699</v>
       </c>
       <c r="C12" t="n">
-        <v>894</v>
+        <v>198</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -613,10 +613,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>798</v>
+        <v>227</v>
       </c>
       <c r="C13" t="n">
-        <v>347</v>
+        <v>254</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -627,10 +627,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>304</v>
+        <v>143</v>
       </c>
       <c r="C14" t="n">
-        <v>803</v>
+        <v>290</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -641,10 +641,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>219</v>
+        <v>780</v>
       </c>
       <c r="C15" t="n">
-        <v>647</v>
+        <v>25</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -655,10 +655,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>945</v>
+        <v>887</v>
       </c>
       <c r="C16" t="n">
-        <v>267</v>
+        <v>327</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -669,10 +669,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>915</v>
+        <v>380</v>
       </c>
       <c r="C17" t="n">
-        <v>944</v>
+        <v>679</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -683,10 +683,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>841</v>
+        <v>25</v>
       </c>
       <c r="C18" t="n">
-        <v>629</v>
+        <v>222</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -697,10 +697,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>314</v>
+        <v>908</v>
       </c>
       <c r="C19" t="n">
-        <v>105</v>
+        <v>828</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -711,10 +711,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="C20" t="n">
-        <v>557</v>
+        <v>887</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
@@ -725,10 +725,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>240</v>
+        <v>437</v>
       </c>
       <c r="C21" t="n">
-        <v>988</v>
+        <v>916</v>
       </c>
       <c r="D21" t="n">
         <v>31</v>
@@ -739,10 +739,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="C22" t="n">
-        <v>61</v>
+        <v>197</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -753,10 +753,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>676</v>
+        <v>564</v>
       </c>
       <c r="C23" t="n">
-        <v>888</v>
+        <v>218</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -767,10 +767,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>554</v>
+        <v>71</v>
       </c>
       <c r="C24" t="n">
-        <v>793</v>
+        <v>345</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -781,10 +781,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>722</v>
+        <v>370</v>
       </c>
       <c r="C25" t="n">
-        <v>801</v>
+        <v>205</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
@@ -795,10 +795,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>132</v>
+        <v>353</v>
       </c>
       <c r="C26" t="n">
-        <v>109</v>
+        <v>505</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
@@ -809,10 +809,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>651</v>
+        <v>775</v>
       </c>
       <c r="C27" t="n">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -823,10 +823,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>14</v>
+        <v>429</v>
       </c>
       <c r="C28" t="n">
-        <v>125</v>
+        <v>276</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
@@ -837,10 +837,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>372</v>
+        <v>769</v>
       </c>
       <c r="C29" t="n">
-        <v>764</v>
+        <v>332</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
@@ -851,10 +851,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>278</v>
+        <v>710</v>
       </c>
       <c r="C30" t="n">
-        <v>955</v>
+        <v>438</v>
       </c>
       <c r="D30" t="n">
         <v>6</v>
@@ -865,10 +865,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>754</v>
+        <v>867</v>
       </c>
       <c r="C31" t="n">
-        <v>582</v>
+        <v>411</v>
       </c>
       <c r="D31" t="n">
         <v>1</v>
@@ -879,10 +879,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>471</v>
+        <v>912</v>
       </c>
       <c r="C32" t="n">
-        <v>97</v>
+        <v>938</v>
       </c>
       <c r="D32" t="n">
         <v>1</v>
@@ -893,10 +893,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="C33" t="n">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
@@ -907,10 +907,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>987</v>
+        <v>498</v>
       </c>
       <c r="C34" t="n">
-        <v>864</v>
+        <v>955</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
@@ -921,10 +921,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>672</v>
+        <v>295</v>
       </c>
       <c r="C35" t="n">
-        <v>200</v>
+        <v>693</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -935,10 +935,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>514</v>
+        <v>744</v>
       </c>
       <c r="C36" t="n">
-        <v>606</v>
+        <v>175</v>
       </c>
       <c r="D36" t="n">
         <v>1</v>
@@ -949,10 +949,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>996</v>
+        <v>185</v>
       </c>
       <c r="C37" t="n">
-        <v>308</v>
+        <v>678</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
@@ -963,10 +963,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>803</v>
+        <v>176</v>
       </c>
       <c r="C38" t="n">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
@@ -977,10 +977,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>617</v>
+        <v>847</v>
       </c>
       <c r="C39" t="n">
-        <v>65</v>
+        <v>964</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
@@ -991,10 +991,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C40" t="n">
-        <v>973</v>
+        <v>684</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
@@ -1005,10 +1005,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>191</v>
+        <v>611</v>
       </c>
       <c r="C41" t="n">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
@@ -1019,10 +1019,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>59</v>
+        <v>681</v>
       </c>
       <c r="C42" t="n">
-        <v>342</v>
+        <v>215</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
@@ -1033,10 +1033,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>535</v>
+        <v>305</v>
       </c>
       <c r="C43" t="n">
-        <v>23</v>
+        <v>427</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
@@ -1047,10 +1047,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>227</v>
+        <v>255</v>
       </c>
       <c r="C44" t="n">
-        <v>332</v>
+        <v>81</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
@@ -1061,10 +1061,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>291</v>
+        <v>632</v>
       </c>
       <c r="C45" t="n">
-        <v>821</v>
+        <v>311</v>
       </c>
       <c r="D45" t="n">
         <v>2</v>
@@ -1075,10 +1075,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>637</v>
+        <v>520</v>
       </c>
       <c r="C46" t="n">
-        <v>959</v>
+        <v>872</v>
       </c>
       <c r="D46" t="n">
         <v>2</v>
@@ -1089,10 +1089,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>860</v>
+        <v>38</v>
       </c>
       <c r="C47" t="n">
-        <v>112</v>
+        <v>349</v>
       </c>
       <c r="D47" t="n">
         <v>2</v>
@@ -1103,10 +1103,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>47</v>
+        <v>493</v>
       </c>
       <c r="C48" t="n">
-        <v>975</v>
+        <v>556</v>
       </c>
       <c r="D48" t="n">
         <v>2</v>
@@ -1117,10 +1117,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>397</v>
+        <v>911</v>
       </c>
       <c r="C49" t="n">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D49" t="n">
         <v>7</v>
@@ -1131,10 +1131,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>871</v>
+        <v>220</v>
       </c>
       <c r="C50" t="n">
-        <v>761</v>
+        <v>972</v>
       </c>
       <c r="D50" t="n">
         <v>2</v>
@@ -1145,10 +1145,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>849</v>
+        <v>783</v>
       </c>
       <c r="C51" t="n">
-        <v>777</v>
+        <v>719</v>
       </c>
       <c r="D51" t="n">
         <v>2</v>
@@ -1159,10 +1159,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>741</v>
+        <v>723</v>
       </c>
       <c r="C52" t="n">
-        <v>575</v>
+        <v>18</v>
       </c>
       <c r="D52" t="n">
         <v>2</v>
@@ -1173,10 +1173,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>572</v>
+        <v>172</v>
       </c>
       <c r="C53" t="n">
-        <v>330</v>
+        <v>991</v>
       </c>
       <c r="D53" t="n">
         <v>2</v>
@@ -1187,10 +1187,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>458</v>
+        <v>804</v>
       </c>
       <c r="C54" t="n">
-        <v>290</v>
+        <v>874</v>
       </c>
       <c r="D54" t="n">
         <v>2</v>
@@ -1201,10 +1201,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C55" t="n">
-        <v>365</v>
+        <v>635</v>
       </c>
       <c r="D55" t="n">
         <v>2</v>
@@ -1215,10 +1215,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>244</v>
+        <v>862</v>
       </c>
       <c r="C56" t="n">
-        <v>655</v>
+        <v>679</v>
       </c>
       <c r="D56" t="n">
         <v>2</v>
@@ -1229,10 +1229,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>234</v>
+        <v>694</v>
       </c>
       <c r="C57" t="n">
-        <v>597</v>
+        <v>121</v>
       </c>
       <c r="D57" t="n">
         <v>2</v>
@@ -1243,10 +1243,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>162</v>
+        <v>482</v>
       </c>
       <c r="C58" t="n">
-        <v>913</v>
+        <v>981</v>
       </c>
       <c r="D58" t="n">
         <v>2</v>
@@ -1257,10 +1257,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C59" t="n">
-        <v>992</v>
+        <v>367</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -1271,10 +1271,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>289</v>
+        <v>530</v>
       </c>
       <c r="C60" t="n">
-        <v>21</v>
+        <v>341</v>
       </c>
       <c r="D60" t="n">
         <v>1</v>
@@ -1285,10 +1285,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>721</v>
+        <v>29</v>
       </c>
       <c r="C61" t="n">
-        <v>652</v>
+        <v>767</v>
       </c>
       <c r="D61" t="n">
         <v>53</v>
@@ -1299,10 +1299,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>934</v>
+        <v>421</v>
       </c>
       <c r="C62" t="n">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="D62" t="n">
         <v>1</v>
@@ -1313,10 +1313,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>299</v>
+        <v>998</v>
       </c>
       <c r="C63" t="n">
-        <v>782</v>
+        <v>705</v>
       </c>
       <c r="D63" t="n">
         <v>1</v>
@@ -1327,10 +1327,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>383</v>
+        <v>315</v>
       </c>
       <c r="C64" t="n">
-        <v>101</v>
+        <v>591</v>
       </c>
       <c r="D64" t="n">
         <v>1</v>
@@ -1341,10 +1341,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>416</v>
+        <v>8</v>
       </c>
       <c r="C65" t="n">
-        <v>921</v>
+        <v>141</v>
       </c>
       <c r="D65" t="n">
         <v>1</v>
@@ -1355,10 +1355,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>822</v>
+        <v>972</v>
       </c>
       <c r="C66" t="n">
-        <v>522</v>
+        <v>881</v>
       </c>
       <c r="D66" t="n">
         <v>1</v>
@@ -1369,10 +1369,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>451</v>
+        <v>531</v>
       </c>
       <c r="C67" t="n">
-        <v>577</v>
+        <v>312</v>
       </c>
       <c r="D67" t="n">
         <v>1</v>
@@ -1383,10 +1383,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>463</v>
+        <v>575</v>
       </c>
       <c r="C68" t="n">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="D68" t="n">
         <v>1</v>
@@ -1397,10 +1397,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>986</v>
+        <v>332</v>
       </c>
       <c r="C69" t="n">
-        <v>528</v>
+        <v>365</v>
       </c>
       <c r="D69" t="n">
         <v>1</v>
@@ -1411,10 +1411,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>542</v>
+        <v>237</v>
       </c>
       <c r="C70" t="n">
-        <v>218</v>
+        <v>778</v>
       </c>
       <c r="D70" t="n">
         <v>1</v>
@@ -1425,10 +1425,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>239</v>
+        <v>617</v>
       </c>
       <c r="C71" t="n">
-        <v>870</v>
+        <v>204</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -1439,10 +1439,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>485</v>
+        <v>677</v>
       </c>
       <c r="C72" t="n">
-        <v>819</v>
+        <v>796</v>
       </c>
       <c r="D72" t="n">
         <v>1</v>
@@ -1453,10 +1453,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>589</v>
+        <v>249</v>
       </c>
       <c r="C73" t="n">
-        <v>466</v>
+        <v>147</v>
       </c>
       <c r="D73" t="n">
         <v>1</v>
@@ -1467,10 +1467,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>584</v>
+        <v>77</v>
       </c>
       <c r="C74" t="n">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
@@ -1481,10 +1481,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>322</v>
+        <v>878</v>
       </c>
       <c r="C75" t="n">
-        <v>511</v>
+        <v>984</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
@@ -1495,10 +1495,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>200</v>
+        <v>325</v>
       </c>
       <c r="C76" t="n">
-        <v>134</v>
+        <v>569</v>
       </c>
       <c r="D76" t="n">
         <v>1</v>
@@ -1509,10 +1509,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>364</v>
+        <v>468</v>
       </c>
       <c r="D77" t="n">
         <v>1</v>
@@ -1523,10 +1523,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>700</v>
+        <v>117</v>
       </c>
       <c r="C78" t="n">
-        <v>645</v>
+        <v>21</v>
       </c>
       <c r="D78" t="n">
         <v>1</v>
@@ -1537,10 +1537,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>598</v>
+        <v>786</v>
       </c>
       <c r="C79" t="n">
-        <v>588</v>
+        <v>406</v>
       </c>
       <c r="D79" t="n">
         <v>1</v>
@@ -1551,10 +1551,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>716</v>
+        <v>201</v>
       </c>
       <c r="C80" t="n">
-        <v>343</v>
+        <v>866</v>
       </c>
       <c r="D80" t="n">
         <v>1</v>
@@ -1565,10 +1565,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>210</v>
+        <v>963</v>
       </c>
       <c r="C81" t="n">
-        <v>190</v>
+        <v>242</v>
       </c>
       <c r="D81" t="n">
         <v>1</v>
@@ -1579,10 +1579,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>535</v>
+        <v>444</v>
       </c>
       <c r="C82" t="n">
-        <v>865</v>
+        <v>161</v>
       </c>
       <c r="D82" t="n">
         <v>1</v>
@@ -1593,10 +1593,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>177</v>
+        <v>746</v>
       </c>
       <c r="C83" t="n">
-        <v>40</v>
+        <v>942</v>
       </c>
       <c r="D83" t="n">
         <v>1</v>
@@ -1607,10 +1607,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>676</v>
+        <v>540</v>
       </c>
       <c r="C84" t="n">
-        <v>483</v>
+        <v>963</v>
       </c>
       <c r="D84" t="n">
         <v>1</v>
@@ -1621,10 +1621,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>812</v>
+        <v>413</v>
       </c>
       <c r="C85" t="n">
-        <v>749</v>
+        <v>712</v>
       </c>
       <c r="D85" t="n">
         <v>1</v>
@@ -1635,10 +1635,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>280</v>
+        <v>858</v>
       </c>
       <c r="C86" t="n">
-        <v>828</v>
+        <v>951</v>
       </c>
       <c r="D86" t="n">
         <v>1</v>
@@ -1649,10 +1649,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>792</v>
+        <v>511</v>
       </c>
       <c r="C87" t="n">
-        <v>213</v>
+        <v>636</v>
       </c>
       <c r="D87" t="n">
         <v>1</v>
@@ -1663,10 +1663,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>78</v>
+        <v>921</v>
       </c>
       <c r="C88" t="n">
-        <v>599</v>
+        <v>213</v>
       </c>
       <c r="D88" t="n">
         <v>1</v>
@@ -1677,10 +1677,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>729</v>
+        <v>263</v>
       </c>
       <c r="C89" t="n">
-        <v>615</v>
+        <v>33</v>
       </c>
       <c r="D89" t="n">
         <v>53</v>
@@ -1691,10 +1691,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>809</v>
+        <v>741</v>
       </c>
       <c r="C90" t="n">
-        <v>297</v>
+        <v>145</v>
       </c>
       <c r="D90" t="n">
         <v>1</v>
@@ -1705,10 +1705,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>167</v>
+        <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>372</v>
+        <v>934</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
@@ -1719,10 +1719,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>479</v>
+        <v>976</v>
       </c>
       <c r="C92" t="n">
-        <v>830</v>
+        <v>280</v>
       </c>
       <c r="D92" t="n">
         <v>1</v>
@@ -1733,10 +1733,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>555</v>
+        <v>801</v>
       </c>
       <c r="C93" t="n">
-        <v>938</v>
+        <v>287</v>
       </c>
       <c r="D93" t="n">
         <v>5</v>
@@ -1747,10 +1747,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>753</v>
+        <v>314</v>
       </c>
       <c r="C94" t="n">
-        <v>358</v>
+        <v>448</v>
       </c>
       <c r="D94" t="n">
         <v>5</v>
@@ -1761,10 +1761,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>870</v>
+        <v>355</v>
       </c>
       <c r="C95" t="n">
-        <v>816</v>
+        <v>648</v>
       </c>
       <c r="D95" t="n">
         <v>5</v>
@@ -1775,10 +1775,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>909</v>
+        <v>863</v>
       </c>
       <c r="C96" t="n">
-        <v>326</v>
+        <v>907</v>
       </c>
       <c r="D96" t="n">
         <v>5</v>
@@ -1789,10 +1789,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>818</v>
+        <v>1000</v>
       </c>
       <c r="C97" t="n">
-        <v>287</v>
+        <v>219</v>
       </c>
       <c r="D97" t="n">
         <v>5</v>
@@ -1803,10 +1803,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>946</v>
+        <v>737</v>
       </c>
       <c r="C98" t="n">
-        <v>918</v>
+        <v>381</v>
       </c>
       <c r="D98" t="n">
         <v>51</v>
@@ -1817,10 +1817,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>718</v>
+        <v>165</v>
       </c>
       <c r="C99" t="n">
-        <v>252</v>
+        <v>708</v>
       </c>
       <c r="D99" t="n">
         <v>5</v>
@@ -1831,10 +1831,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>473</v>
+        <v>95</v>
       </c>
       <c r="C100" t="n">
-        <v>633</v>
+        <v>856</v>
       </c>
       <c r="D100" t="n">
         <v>35</v>
@@ -1845,10 +1845,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>311</v>
+        <v>524</v>
       </c>
       <c r="C101" t="n">
-        <v>108</v>
+        <v>734</v>
       </c>
       <c r="D101" t="n">
         <v>11</v>
@@ -1865,7 +1865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1890,333 +1890,351 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B2" t="n">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>96</v>
+        <v>43</v>
+      </c>
+      <c r="D2" t="n">
+        <v>47</v>
       </c>
       <c r="E2" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F2" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G2" t="n">
-        <v>76</v>
-      </c>
-      <c r="H2" t="n">
-        <v>15</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B3" t="n">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="C3" t="n">
-        <v>95</v>
+        <v>72</v>
+      </c>
+      <c r="D3" t="n">
+        <v>86</v>
       </c>
       <c r="E3" t="n">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="F3" t="n">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="G3" t="n">
-        <v>54</v>
-      </c>
-      <c r="H3" t="n">
-        <v>86</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B4" t="n">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>77</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F4" t="n">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G4" t="n">
-        <v>87</v>
-      </c>
-      <c r="H4" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C5" t="n">
-        <v>98</v>
+        <v>32</v>
+      </c>
+      <c r="D5" t="n">
+        <v>51</v>
       </c>
       <c r="E5" t="n">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="G5" t="n">
-        <v>56</v>
-      </c>
-      <c r="H5" t="n">
-        <v>36</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B6" t="n">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="C6" t="n">
+        <v>24</v>
       </c>
       <c r="E6" t="n">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="F6" t="n">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="G6" t="n">
-        <v>74</v>
-      </c>
-      <c r="H6" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" t="n">
-        <v>67</v>
+        <v>90</v>
+      </c>
+      <c r="C7" t="n">
+        <v>81</v>
       </c>
       <c r="E7" t="n">
-        <v>39</v>
-      </c>
-      <c r="F7" t="n">
-        <v>40</v>
+        <v>100</v>
+      </c>
+      <c r="G7" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>48</v>
+      </c>
+      <c r="B8" t="n">
+        <v>36</v>
+      </c>
+      <c r="C8" t="n">
+        <v>12</v>
+      </c>
+      <c r="E8" t="n">
         <v>84</v>
-      </c>
-      <c r="B8" t="n">
-        <v>66</v>
-      </c>
-      <c r="E8" t="n">
-        <v>64</v>
-      </c>
-      <c r="F8" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B9" t="n">
+        <v>79</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
         <v>71</v>
-      </c>
-      <c r="E9" t="n">
-        <v>47</v>
-      </c>
-      <c r="F9" t="n">
-        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="B10" t="n">
-        <v>19</v>
+        <v>69</v>
+      </c>
+      <c r="C10" t="n">
+        <v>21</v>
       </c>
       <c r="E10" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" t="n">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B11" t="n">
-        <v>93</v>
+        <v>52</v>
+      </c>
+      <c r="C11" t="n">
+        <v>64</v>
       </c>
       <c r="E11" t="n">
-        <v>11</v>
-      </c>
-      <c r="F11" t="n">
-        <v>25</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B12" t="n">
-        <v>73</v>
+        <v>34</v>
+      </c>
+      <c r="C12" t="n">
+        <v>37</v>
       </c>
       <c r="E12" t="n">
-        <v>62</v>
-      </c>
-      <c r="F12" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="B13" t="n">
-        <v>91</v>
+        <v>49</v>
+      </c>
+      <c r="C13" t="n">
+        <v>13</v>
       </c>
       <c r="E13" t="n">
-        <v>58</v>
-      </c>
-      <c r="F13" t="n">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>79</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" t="n">
-        <v>53</v>
+        <v>76</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B15" t="n">
-        <v>12</v>
-      </c>
-      <c r="E15" t="n">
-        <v>55</v>
-      </c>
-      <c r="F15" t="n">
-        <v>43</v>
+        <v>63</v>
+      </c>
+      <c r="C15" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B16" t="n">
-        <v>37</v>
-      </c>
-      <c r="E16" t="n">
-        <v>14</v>
-      </c>
-      <c r="F16" t="n">
-        <v>42</v>
+        <v>3</v>
+      </c>
+      <c r="C16" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B17" t="n">
-        <v>48</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4</v>
+        <v>94</v>
+      </c>
+      <c r="C17" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B18" t="n">
-        <v>52</v>
-      </c>
-      <c r="F18" t="n">
-        <v>69</v>
+        <v>75</v>
+      </c>
+      <c r="C18" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B19" t="n">
-        <v>89</v>
-      </c>
-      <c r="F19" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" t="n">
-        <v>28</v>
-      </c>
-      <c r="F20" t="n">
-        <v>90</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>65</v>
-      </c>
-      <c r="F21" t="n">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>9</v>
-      </c>
-      <c r="F22" t="n">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>68</v>
-      </c>
-      <c r="F23" t="n">
-        <v>41</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   InitialTopo.py 	modified:   Main.py 	modified:   __pycache__/InitialTopo.cpython-310.pyc 	modified:   __pycache__/Mentor_2.cpython-310.pyc 	modified:   mentor2_result.txt 	modified:   nodes_inf.xlsx
</commit_message>
<xml_diff>
--- a/nodes_inf.xlsx
+++ b/nodes_inf.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Node Info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Backbones" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Backbones1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,10 +460,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>518</v>
+        <v>673</v>
       </c>
       <c r="C2" t="n">
-        <v>59</v>
+        <v>855</v>
       </c>
       <c r="D2" t="n">
         <v>11</v>
@@ -473,10 +474,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>790</v>
+        <v>510</v>
       </c>
       <c r="C3" t="n">
-        <v>840</v>
+        <v>861</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -487,10 +488,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>96</v>
+        <v>472</v>
       </c>
       <c r="C4" t="n">
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
@@ -501,10 +502,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>882</v>
+        <v>334</v>
       </c>
       <c r="C5" t="n">
-        <v>598</v>
+        <v>946</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
@@ -515,10 +516,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>95</v>
+        <v>868</v>
       </c>
       <c r="C6" t="n">
-        <v>742</v>
+        <v>963</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
@@ -529,10 +530,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>502</v>
+        <v>359</v>
       </c>
       <c r="C7" t="n">
-        <v>186</v>
+        <v>731</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
@@ -543,10 +544,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>492</v>
+        <v>853</v>
       </c>
       <c r="C8" t="n">
-        <v>645</v>
+        <v>577</v>
       </c>
       <c r="D8" t="n">
         <v>5</v>
@@ -557,10 +558,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>829</v>
+        <v>394</v>
       </c>
       <c r="C9" t="n">
-        <v>389</v>
+        <v>687</v>
       </c>
       <c r="D9" t="n">
         <v>51</v>
@@ -571,10 +572,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>787</v>
+        <v>869</v>
       </c>
       <c r="C10" t="n">
-        <v>168</v>
+        <v>333</v>
       </c>
       <c r="D10" t="n">
         <v>5</v>
@@ -585,10 +586,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>604</v>
+        <v>906</v>
       </c>
       <c r="C11" t="n">
-        <v>201</v>
+        <v>118</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -599,10 +600,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>699</v>
+        <v>886</v>
       </c>
       <c r="C12" t="n">
-        <v>198</v>
+        <v>253</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -613,10 +614,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>227</v>
+        <v>727</v>
       </c>
       <c r="C13" t="n">
-        <v>254</v>
+        <v>462</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -627,10 +628,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>143</v>
+        <v>749</v>
       </c>
       <c r="C14" t="n">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -641,10 +642,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>780</v>
+        <v>120</v>
       </c>
       <c r="C15" t="n">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -655,10 +656,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>887</v>
+        <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>327</v>
+        <v>190</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -669,10 +670,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>380</v>
+        <v>222</v>
       </c>
       <c r="C17" t="n">
-        <v>679</v>
+        <v>493</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -683,10 +684,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>25</v>
+        <v>243</v>
       </c>
       <c r="C18" t="n">
-        <v>222</v>
+        <v>855</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -697,10 +698,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>908</v>
+        <v>774</v>
       </c>
       <c r="C19" t="n">
-        <v>828</v>
+        <v>936</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -711,10 +712,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>470</v>
+        <v>338</v>
       </c>
       <c r="C20" t="n">
-        <v>887</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
@@ -725,10 +726,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>437</v>
+        <v>37</v>
       </c>
       <c r="C21" t="n">
-        <v>916</v>
+        <v>729</v>
       </c>
       <c r="D21" t="n">
         <v>31</v>
@@ -739,10 +740,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>59</v>
+        <v>757</v>
       </c>
       <c r="C22" t="n">
-        <v>197</v>
+        <v>756</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -753,10 +754,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>564</v>
+        <v>190</v>
       </c>
       <c r="C23" t="n">
-        <v>218</v>
+        <v>518</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -767,10 +768,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>71</v>
+        <v>398</v>
       </c>
       <c r="C24" t="n">
-        <v>345</v>
+        <v>772</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -781,10 +782,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>370</v>
+        <v>607</v>
       </c>
       <c r="C25" t="n">
-        <v>205</v>
+        <v>824</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
@@ -795,10 +796,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>353</v>
+        <v>13</v>
       </c>
       <c r="C26" t="n">
-        <v>505</v>
+        <v>103</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
@@ -809,10 +810,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>775</v>
+        <v>812</v>
       </c>
       <c r="C27" t="n">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -823,10 +824,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>429</v>
+        <v>903</v>
       </c>
       <c r="C28" t="n">
-        <v>276</v>
+        <v>602</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
@@ -837,10 +838,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>769</v>
+        <v>419</v>
       </c>
       <c r="C29" t="n">
-        <v>332</v>
+        <v>512</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
@@ -851,10 +852,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>710</v>
+        <v>977</v>
       </c>
       <c r="C30" t="n">
-        <v>438</v>
+        <v>220</v>
       </c>
       <c r="D30" t="n">
         <v>6</v>
@@ -865,10 +866,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>867</v>
+        <v>462</v>
       </c>
       <c r="C31" t="n">
-        <v>411</v>
+        <v>899</v>
       </c>
       <c r="D31" t="n">
         <v>1</v>
@@ -879,10 +880,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>912</v>
+        <v>209</v>
       </c>
       <c r="C32" t="n">
-        <v>938</v>
+        <v>532</v>
       </c>
       <c r="D32" t="n">
         <v>1</v>
@@ -893,10 +894,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>117</v>
+        <v>914</v>
       </c>
       <c r="C33" t="n">
-        <v>16</v>
+        <v>536</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
@@ -907,10 +908,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>498</v>
+        <v>414</v>
       </c>
       <c r="C34" t="n">
-        <v>955</v>
+        <v>87</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
@@ -921,10 +922,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>295</v>
+        <v>842</v>
       </c>
       <c r="C35" t="n">
-        <v>693</v>
+        <v>328</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -935,10 +936,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>744</v>
+        <v>195</v>
       </c>
       <c r="C36" t="n">
-        <v>175</v>
+        <v>834</v>
       </c>
       <c r="D36" t="n">
         <v>1</v>
@@ -949,10 +950,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>185</v>
+        <v>966</v>
       </c>
       <c r="C37" t="n">
-        <v>678</v>
+        <v>689</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
@@ -963,10 +964,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="C38" t="n">
-        <v>297</v>
+        <v>140</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
@@ -977,10 +978,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>847</v>
+        <v>30</v>
       </c>
       <c r="C39" t="n">
-        <v>964</v>
+        <v>864</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
@@ -991,10 +992,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>47</v>
+        <v>508</v>
       </c>
       <c r="C40" t="n">
-        <v>684</v>
+        <v>916</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
@@ -1005,10 +1006,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>611</v>
+        <v>663</v>
       </c>
       <c r="C41" t="n">
-        <v>176</v>
+        <v>650</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
@@ -1019,10 +1020,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>681</v>
+        <v>387</v>
       </c>
       <c r="C42" t="n">
-        <v>215</v>
+        <v>540</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
@@ -1033,10 +1034,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="C43" t="n">
-        <v>427</v>
+        <v>354</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
@@ -1047,10 +1048,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>255</v>
+        <v>831</v>
       </c>
       <c r="C44" t="n">
-        <v>81</v>
+        <v>885</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
@@ -1061,10 +1062,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>632</v>
+        <v>241</v>
       </c>
       <c r="C45" t="n">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D45" t="n">
         <v>2</v>
@@ -1075,10 +1076,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>520</v>
+        <v>642</v>
       </c>
       <c r="C46" t="n">
-        <v>872</v>
+        <v>836</v>
       </c>
       <c r="D46" t="n">
         <v>2</v>
@@ -1089,10 +1090,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>38</v>
+        <v>209</v>
       </c>
       <c r="C47" t="n">
-        <v>349</v>
+        <v>779</v>
       </c>
       <c r="D47" t="n">
         <v>2</v>
@@ -1103,10 +1104,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>493</v>
+        <v>602</v>
       </c>
       <c r="C48" t="n">
-        <v>556</v>
+        <v>701</v>
       </c>
       <c r="D48" t="n">
         <v>2</v>
@@ -1117,10 +1118,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>911</v>
+        <v>91</v>
       </c>
       <c r="C49" t="n">
-        <v>524</v>
+        <v>479</v>
       </c>
       <c r="D49" t="n">
         <v>7</v>
@@ -1131,10 +1132,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>220</v>
+        <v>345</v>
       </c>
       <c r="C50" t="n">
-        <v>972</v>
+        <v>749</v>
       </c>
       <c r="D50" t="n">
         <v>2</v>
@@ -1145,10 +1146,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>783</v>
+        <v>319</v>
       </c>
       <c r="C51" t="n">
-        <v>719</v>
+        <v>786</v>
       </c>
       <c r="D51" t="n">
         <v>2</v>
@@ -1159,10 +1160,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>723</v>
+        <v>524</v>
       </c>
       <c r="C52" t="n">
-        <v>18</v>
+        <v>832</v>
       </c>
       <c r="D52" t="n">
         <v>2</v>
@@ -1173,10 +1174,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>172</v>
+        <v>570</v>
       </c>
       <c r="C53" t="n">
-        <v>991</v>
+        <v>344</v>
       </c>
       <c r="D53" t="n">
         <v>2</v>
@@ -1187,10 +1188,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>804</v>
+        <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>874</v>
+        <v>935</v>
       </c>
       <c r="D54" t="n">
         <v>2</v>
@@ -1201,10 +1202,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>96</v>
+        <v>402</v>
       </c>
       <c r="C55" t="n">
-        <v>635</v>
+        <v>601</v>
       </c>
       <c r="D55" t="n">
         <v>2</v>
@@ -1215,10 +1216,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>862</v>
+        <v>309</v>
       </c>
       <c r="C56" t="n">
-        <v>679</v>
+        <v>178</v>
       </c>
       <c r="D56" t="n">
         <v>2</v>
@@ -1229,10 +1230,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>694</v>
+        <v>800</v>
       </c>
       <c r="C57" t="n">
-        <v>121</v>
+        <v>274</v>
       </c>
       <c r="D57" t="n">
         <v>2</v>
@@ -1243,10 +1244,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>482</v>
+        <v>530</v>
       </c>
       <c r="C58" t="n">
-        <v>981</v>
+        <v>925</v>
       </c>
       <c r="D58" t="n">
         <v>2</v>
@@ -1257,10 +1258,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>80</v>
+        <v>552</v>
       </c>
       <c r="C59" t="n">
-        <v>367</v>
+        <v>801</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -1271,10 +1272,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>530</v>
+        <v>899</v>
       </c>
       <c r="C60" t="n">
-        <v>341</v>
+        <v>1000</v>
       </c>
       <c r="D60" t="n">
         <v>1</v>
@@ -1285,10 +1286,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>29</v>
+        <v>654</v>
       </c>
       <c r="C61" t="n">
-        <v>767</v>
+        <v>933</v>
       </c>
       <c r="D61" t="n">
         <v>53</v>
@@ -1299,10 +1300,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>421</v>
+        <v>760</v>
       </c>
       <c r="C62" t="n">
-        <v>648</v>
+        <v>333</v>
       </c>
       <c r="D62" t="n">
         <v>1</v>
@@ -1313,10 +1314,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>998</v>
+        <v>150</v>
       </c>
       <c r="C63" t="n">
-        <v>705</v>
+        <v>172</v>
       </c>
       <c r="D63" t="n">
         <v>1</v>
@@ -1327,10 +1328,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>315</v>
+        <v>736</v>
       </c>
       <c r="C64" t="n">
-        <v>591</v>
+        <v>88</v>
       </c>
       <c r="D64" t="n">
         <v>1</v>
@@ -1341,10 +1342,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>8</v>
+        <v>504</v>
       </c>
       <c r="C65" t="n">
-        <v>141</v>
+        <v>747</v>
       </c>
       <c r="D65" t="n">
         <v>1</v>
@@ -1355,10 +1356,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>972</v>
+        <v>687</v>
       </c>
       <c r="C66" t="n">
-        <v>881</v>
+        <v>911</v>
       </c>
       <c r="D66" t="n">
         <v>1</v>
@@ -1369,10 +1370,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>531</v>
+        <v>476</v>
       </c>
       <c r="C67" t="n">
-        <v>312</v>
+        <v>505</v>
       </c>
       <c r="D67" t="n">
         <v>1</v>
@@ -1383,10 +1384,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>575</v>
+        <v>914</v>
       </c>
       <c r="C68" t="n">
-        <v>560</v>
+        <v>935</v>
       </c>
       <c r="D68" t="n">
         <v>1</v>
@@ -1397,10 +1398,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>332</v>
+        <v>756</v>
       </c>
       <c r="C69" t="n">
-        <v>365</v>
+        <v>636</v>
       </c>
       <c r="D69" t="n">
         <v>1</v>
@@ -1411,10 +1412,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>237</v>
+        <v>352</v>
       </c>
       <c r="C70" t="n">
-        <v>778</v>
+        <v>210</v>
       </c>
       <c r="D70" t="n">
         <v>1</v>
@@ -1425,10 +1426,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>617</v>
+        <v>374</v>
       </c>
       <c r="C71" t="n">
-        <v>204</v>
+        <v>883</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -1439,10 +1440,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>677</v>
+        <v>366</v>
       </c>
       <c r="C72" t="n">
-        <v>796</v>
+        <v>156</v>
       </c>
       <c r="D72" t="n">
         <v>1</v>
@@ -1453,10 +1454,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>249</v>
+        <v>507</v>
       </c>
       <c r="C73" t="n">
-        <v>147</v>
+        <v>368</v>
       </c>
       <c r="D73" t="n">
         <v>1</v>
@@ -1467,10 +1468,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>77</v>
+        <v>985</v>
       </c>
       <c r="C74" t="n">
-        <v>390</v>
+        <v>621</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
@@ -1481,10 +1482,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>878</v>
+        <v>556</v>
       </c>
       <c r="C75" t="n">
-        <v>984</v>
+        <v>661</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
@@ -1495,10 +1496,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>325</v>
+        <v>170</v>
       </c>
       <c r="C76" t="n">
-        <v>569</v>
+        <v>660</v>
       </c>
       <c r="D76" t="n">
         <v>1</v>
@@ -1509,10 +1510,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>10</v>
+        <v>842</v>
       </c>
       <c r="C77" t="n">
-        <v>468</v>
+        <v>69</v>
       </c>
       <c r="D77" t="n">
         <v>1</v>
@@ -1523,10 +1524,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>117</v>
+        <v>286</v>
       </c>
       <c r="C78" t="n">
-        <v>21</v>
+        <v>154</v>
       </c>
       <c r="D78" t="n">
         <v>1</v>
@@ -1537,10 +1538,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>786</v>
+        <v>595</v>
       </c>
       <c r="C79" t="n">
-        <v>406</v>
+        <v>489</v>
       </c>
       <c r="D79" t="n">
         <v>1</v>
@@ -1551,10 +1552,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="C80" t="n">
-        <v>866</v>
+        <v>828</v>
       </c>
       <c r="D80" t="n">
         <v>1</v>
@@ -1565,10 +1566,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>963</v>
+        <v>540</v>
       </c>
       <c r="C81" t="n">
-        <v>242</v>
+        <v>294</v>
       </c>
       <c r="D81" t="n">
         <v>1</v>
@@ -1579,10 +1580,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>444</v>
+        <v>828</v>
       </c>
       <c r="C82" t="n">
-        <v>161</v>
+        <v>4</v>
       </c>
       <c r="D82" t="n">
         <v>1</v>
@@ -1593,10 +1594,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>746</v>
+        <v>876</v>
       </c>
       <c r="C83" t="n">
-        <v>942</v>
+        <v>635</v>
       </c>
       <c r="D83" t="n">
         <v>1</v>
@@ -1607,10 +1608,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>540</v>
+        <v>760</v>
       </c>
       <c r="C84" t="n">
-        <v>963</v>
+        <v>114</v>
       </c>
       <c r="D84" t="n">
         <v>1</v>
@@ -1621,10 +1622,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>413</v>
+        <v>748</v>
       </c>
       <c r="C85" t="n">
-        <v>712</v>
+        <v>812</v>
       </c>
       <c r="D85" t="n">
         <v>1</v>
@@ -1635,10 +1636,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>858</v>
+        <v>234</v>
       </c>
       <c r="C86" t="n">
-        <v>951</v>
+        <v>212</v>
       </c>
       <c r="D86" t="n">
         <v>1</v>
@@ -1649,10 +1650,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>511</v>
+        <v>355</v>
       </c>
       <c r="C87" t="n">
-        <v>636</v>
+        <v>620</v>
       </c>
       <c r="D87" t="n">
         <v>1</v>
@@ -1663,10 +1664,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>921</v>
+        <v>349</v>
       </c>
       <c r="C88" t="n">
-        <v>213</v>
+        <v>714</v>
       </c>
       <c r="D88" t="n">
         <v>1</v>
@@ -1677,10 +1678,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>263</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>33</v>
+        <v>827</v>
       </c>
       <c r="D89" t="n">
         <v>53</v>
@@ -1691,10 +1692,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>741</v>
+        <v>257</v>
       </c>
       <c r="C90" t="n">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="D90" t="n">
         <v>1</v>
@@ -1705,10 +1706,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C91" t="n">
-        <v>934</v>
+        <v>884</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
@@ -1719,10 +1720,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>976</v>
+        <v>323</v>
       </c>
       <c r="C92" t="n">
-        <v>280</v>
+        <v>201</v>
       </c>
       <c r="D92" t="n">
         <v>1</v>
@@ -1733,10 +1734,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>801</v>
+        <v>414</v>
       </c>
       <c r="C93" t="n">
-        <v>287</v>
+        <v>207</v>
       </c>
       <c r="D93" t="n">
         <v>5</v>
@@ -1747,10 +1748,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>314</v>
+        <v>617</v>
       </c>
       <c r="C94" t="n">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="D94" t="n">
         <v>5</v>
@@ -1761,10 +1762,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>355</v>
+        <v>289</v>
       </c>
       <c r="C95" t="n">
-        <v>648</v>
+        <v>185</v>
       </c>
       <c r="D95" t="n">
         <v>5</v>
@@ -1775,10 +1776,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>863</v>
+        <v>50</v>
       </c>
       <c r="C96" t="n">
-        <v>907</v>
+        <v>452</v>
       </c>
       <c r="D96" t="n">
         <v>5</v>
@@ -1789,10 +1790,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="C97" t="n">
-        <v>219</v>
+        <v>707</v>
       </c>
       <c r="D97" t="n">
         <v>5</v>
@@ -1803,10 +1804,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>737</v>
+        <v>997</v>
       </c>
       <c r="C98" t="n">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="D98" t="n">
         <v>51</v>
@@ -1817,10 +1818,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="C99" t="n">
-        <v>708</v>
+        <v>650</v>
       </c>
       <c r="D99" t="n">
         <v>5</v>
@@ -1831,10 +1832,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="C100" t="n">
-        <v>856</v>
+        <v>56</v>
       </c>
       <c r="D100" t="n">
         <v>35</v>
@@ -1845,10 +1846,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>524</v>
+        <v>138</v>
       </c>
       <c r="C101" t="n">
-        <v>734</v>
+        <v>575</v>
       </c>
       <c r="D101" t="n">
         <v>11</v>
@@ -1865,7 +1866,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,184 +1888,580 @@
         <v>97</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>95</v>
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="D2" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
-      </c>
-      <c r="F2" t="n">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="G2" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C3" t="n">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D3" t="n">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="E3" t="n">
-        <v>33</v>
-      </c>
-      <c r="F3" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="G3" t="n">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B4" t="n">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E4" t="n">
-        <v>57</v>
-      </c>
-      <c r="F4" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G4" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B5" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C5" t="n">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D5" t="n">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F5" t="n">
-        <v>58</v>
-      </c>
-      <c r="G5" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B6" t="n">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C6" t="n">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11</v>
       </c>
       <c r="E6" t="n">
-        <v>83</v>
-      </c>
-      <c r="F6" t="n">
-        <v>46</v>
-      </c>
-      <c r="G6" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B7" t="n">
-        <v>90</v>
-      </c>
-      <c r="C7" t="n">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="D7" t="n">
+        <v>56</v>
       </c>
       <c r="E7" t="n">
-        <v>100</v>
-      </c>
-      <c r="G7" t="n">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>48</v>
-      </c>
-      <c r="B8" t="n">
-        <v>36</v>
-      </c>
-      <c r="C8" t="n">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="D8" t="n">
+        <v>73</v>
       </c>
       <c r="E8" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>91</v>
-      </c>
-      <c r="B9" t="n">
-        <v>79</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="D9" t="n">
+        <v>27</v>
       </c>
       <c r="E9" t="n">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>87</v>
+        <v>41</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>98</v>
+      </c>
+      <c r="D11" t="n">
+        <v>61</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>74</v>
+      </c>
+      <c r="D12" t="n">
+        <v>13</v>
+      </c>
+      <c r="E12" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>28</v>
+      </c>
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>51</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>58</v>
+      </c>
+      <c r="D15" t="n">
+        <v>36</v>
+      </c>
+      <c r="E15" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="D16" t="n">
+        <v>76</v>
+      </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>66</v>
+      </c>
+      <c r="D17" t="n">
+        <v>83</v>
+      </c>
+      <c r="E17" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>46</v>
+      </c>
+      <c r="E18" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>43</v>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>45</v>
+      </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
+      <c r="E2" t="n">
+        <v>49</v>
+      </c>
+      <c r="F2" t="n">
+        <v>19</v>
+      </c>
+      <c r="G2" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>46</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>83</v>
+      </c>
+      <c r="E3" t="n">
+        <v>95</v>
+      </c>
+      <c r="F3" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>50</v>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>48</v>
+      </c>
+      <c r="E4" t="n">
+        <v>61</v>
+      </c>
+      <c r="F4" t="n">
+        <v>74</v>
+      </c>
+      <c r="G4" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>79</v>
+      </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+      <c r="E5" t="n">
+        <v>77</v>
+      </c>
+      <c r="F5" t="n">
+        <v>32</v>
+      </c>
+      <c r="G5" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>55</v>
+      </c>
+      <c r="E6" t="n">
+        <v>66</v>
+      </c>
+      <c r="F6" t="n">
+        <v>69</v>
+      </c>
+      <c r="G6" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>28</v>
+      </c>
+      <c r="B7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>78</v>
+      </c>
+      <c r="G7" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>59</v>
+      </c>
+      <c r="B8" t="n">
+        <v>76</v>
+      </c>
+      <c r="E8" t="n">
+        <v>65</v>
+      </c>
+      <c r="G8" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" t="n">
+        <v>52</v>
+      </c>
+      <c r="E9" t="n">
+        <v>92</v>
+      </c>
+      <c r="G9" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>69</v>
-      </c>
-      <c r="C10" t="n">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E10" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -2072,169 +2469,192 @@
         <v>80</v>
       </c>
       <c r="B11" t="n">
-        <v>52</v>
-      </c>
-      <c r="C11" t="n">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E11" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>34</v>
-      </c>
-      <c r="C12" t="n">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B13" t="n">
-        <v>49</v>
-      </c>
-      <c r="C13" t="n">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="E13" t="n">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>76</v>
-      </c>
-      <c r="C14" t="n">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="E14" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B15" t="n">
-        <v>63</v>
-      </c>
-      <c r="C15" t="n">
-        <v>27</v>
+        <v>42</v>
+      </c>
+      <c r="E15" t="n">
+        <v>89</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
-      </c>
-      <c r="C16" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="B17" t="n">
-        <v>94</v>
-      </c>
-      <c r="C17" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B18" t="n">
-        <v>75</v>
-      </c>
-      <c r="C18" t="n">
-        <v>23</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B19" t="n">
-        <v>16</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="B20" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>70</v>
+        <v>98</v>
+      </c>
+      <c r="B21" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c r="B22" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>10</v>
+        <v>51</v>
+      </c>
+      <c r="B23" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>56</v>
+        <v>30</v>
+      </c>
+      <c r="B24" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>59</v>
+        <v>96</v>
+      </c>
+      <c r="B25" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>40</v>
+        <v>68</v>
+      </c>
+      <c r="B26" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>67</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>62</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>14</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   Main.py 	modified:   nodes_inf.xlsx
</commit_message>
<xml_diff>
--- a/nodes_inf.xlsx
+++ b/nodes_inf.xlsx
@@ -10,6 +10,8 @@
     <sheet name="Node Info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Backbones" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Backbones1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Backbones2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Backbones3" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2660,4 +2662,772 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>81</v>
+      </c>
+      <c r="B2" t="n">
+        <v>53</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44</v>
+      </c>
+      <c r="E2" t="n">
+        <v>42</v>
+      </c>
+      <c r="F2" t="n">
+        <v>38</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>51</v>
+      </c>
+      <c r="B3" t="n">
+        <v>31</v>
+      </c>
+      <c r="C3" t="n">
+        <v>41</v>
+      </c>
+      <c r="D3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E3" t="n">
+        <v>18</v>
+      </c>
+      <c r="F3" t="n">
+        <v>59</v>
+      </c>
+      <c r="G3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>87</v>
+      </c>
+      <c r="B4" t="n">
+        <v>27</v>
+      </c>
+      <c r="C4" t="n">
+        <v>91</v>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>65</v>
+      </c>
+      <c r="F4" t="n">
+        <v>62</v>
+      </c>
+      <c r="G4" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>68</v>
+      </c>
+      <c r="B5" t="n">
+        <v>95</v>
+      </c>
+      <c r="C5" t="n">
+        <v>48</v>
+      </c>
+      <c r="D5" t="n">
+        <v>19</v>
+      </c>
+      <c r="E5" t="n">
+        <v>36</v>
+      </c>
+      <c r="F5" t="n">
+        <v>85</v>
+      </c>
+      <c r="G5" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="n">
+        <v>56</v>
+      </c>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>92</v>
+      </c>
+      <c r="E6" t="n">
+        <v>61</v>
+      </c>
+      <c r="G6" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32</v>
+      </c>
+      <c r="B7" t="n">
+        <v>35</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>54</v>
+      </c>
+      <c r="E7" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" t="n">
+        <v>94</v>
+      </c>
+      <c r="E8" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>73</v>
+      </c>
+      <c r="B9" t="n">
+        <v>49</v>
+      </c>
+      <c r="C9" t="n">
+        <v>69</v>
+      </c>
+      <c r="D9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>82</v>
+      </c>
+      <c r="B10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C10" t="n">
+        <v>64</v>
+      </c>
+      <c r="D10" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" t="n">
+        <v>34</v>
+      </c>
+      <c r="C11" t="n">
+        <v>96</v>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>90</v>
+      </c>
+      <c r="B12" t="n">
+        <v>78</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>50</v>
+      </c>
+      <c r="B13" t="n">
+        <v>93</v>
+      </c>
+      <c r="C13" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>22</v>
+      </c>
+      <c r="B14" t="n">
+        <v>67</v>
+      </c>
+      <c r="C14" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>76</v>
+      </c>
+      <c r="B15" t="n">
+        <v>46</v>
+      </c>
+      <c r="C15" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>20</v>
+      </c>
+      <c r="B16" t="n">
+        <v>23</v>
+      </c>
+      <c r="C16" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>55</v>
+      </c>
+      <c r="C17" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>70</v>
+      </c>
+      <c r="B18" t="n">
+        <v>74</v>
+      </c>
+      <c r="C18" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>47</v>
+      </c>
+      <c r="B19" t="n">
+        <v>80</v>
+      </c>
+      <c r="C19" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>45</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>13</v>
+      </c>
+      <c r="B21" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>55</v>
+      </c>
+      <c r="B2" t="n">
+        <v>42</v>
+      </c>
+      <c r="D2" t="n">
+        <v>37</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40</v>
+      </c>
+      <c r="F2" t="n">
+        <v>47</v>
+      </c>
+      <c r="G2" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>91</v>
+      </c>
+      <c r="B3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>86</v>
+      </c>
+      <c r="E3" t="n">
+        <v>38</v>
+      </c>
+      <c r="F3" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B4" t="n">
+        <v>29</v>
+      </c>
+      <c r="D4" t="n">
+        <v>77</v>
+      </c>
+      <c r="E4" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>36</v>
+      </c>
+      <c r="B5" t="n">
+        <v>24</v>
+      </c>
+      <c r="D5" t="n">
+        <v>93</v>
+      </c>
+      <c r="E5" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B6" t="n">
+        <v>72</v>
+      </c>
+      <c r="D6" t="n">
+        <v>98</v>
+      </c>
+      <c r="E6" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>21</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>66</v>
+      </c>
+      <c r="B8" t="n">
+        <v>59</v>
+      </c>
+      <c r="D8" t="n">
+        <v>92</v>
+      </c>
+      <c r="E8" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>28</v>
+      </c>
+      <c r="B9" t="n">
+        <v>70</v>
+      </c>
+      <c r="D9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E9" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>68</v>
+      </c>
+      <c r="E10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>75</v>
+      </c>
+      <c r="B11" t="n">
+        <v>73</v>
+      </c>
+      <c r="D11" t="n">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>35</v>
+      </c>
+      <c r="B12" t="n">
+        <v>61</v>
+      </c>
+      <c r="D12" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>81</v>
+      </c>
+      <c r="B13" t="n">
+        <v>16</v>
+      </c>
+      <c r="D13" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>46</v>
+      </c>
+      <c r="B15" t="n">
+        <v>84</v>
+      </c>
+      <c r="D15" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>57</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>85</v>
+      </c>
+      <c r="B17" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>19</v>
+      </c>
+      <c r="B18" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>56</v>
+      </c>
+      <c r="B19" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>41</v>
+      </c>
+      <c r="B20" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>99</v>
+      </c>
+      <c r="B21" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>23</v>
+      </c>
+      <c r="B22" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>80</v>
+      </c>
+      <c r="B23" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>67</v>
+      </c>
+      <c r="B24" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>49</v>
+      </c>
+      <c r="B25" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>44</v>
+      </c>
+      <c r="B26" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>52</v>
+      </c>
+      <c r="B27" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>100</v>
+      </c>
+      <c r="B28" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>14</v>
+      </c>
+      <c r="B29" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>39</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>87</v>
+      </c>
+      <c r="B31" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   MENTOR.py 	modified:   Mentor_2.py 	modified:   __pycache__/MENTOR.cpython-310.pyc 	modified:   __pycache__/Mentor_2.cpython-310.pyc 	modified:   nodes_inf.xlsx
</commit_message>
<xml_diff>
--- a/nodes_inf.xlsx
+++ b/nodes_inf.xlsx
@@ -12,6 +12,11 @@
     <sheet name="Backbones1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Backbones2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Backbones3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Backbones4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Backbones5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Backbones6" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Backbones7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Backbones8" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1862,6 +1867,385 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>59</v>
+      </c>
+      <c r="B2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E2" t="n">
+        <v>69</v>
+      </c>
+      <c r="F2" t="n">
+        <v>62</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>70</v>
+      </c>
+      <c r="C3" t="n">
+        <v>52</v>
+      </c>
+      <c r="D3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E3" t="n">
+        <v>61</v>
+      </c>
+      <c r="F3" t="n">
+        <v>81</v>
+      </c>
+      <c r="G3" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>49</v>
+      </c>
+      <c r="B4" t="n">
+        <v>41</v>
+      </c>
+      <c r="D4" t="n">
+        <v>56</v>
+      </c>
+      <c r="E4" t="n">
+        <v>72</v>
+      </c>
+      <c r="F4" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>76</v>
+      </c>
+      <c r="B5" t="n">
+        <v>66</v>
+      </c>
+      <c r="D5" t="n">
+        <v>39</v>
+      </c>
+      <c r="E5" t="n">
+        <v>73</v>
+      </c>
+      <c r="F5" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>86</v>
+      </c>
+      <c r="B6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93</v>
+      </c>
+      <c r="E6" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>95</v>
+      </c>
+      <c r="B7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" t="n">
+        <v>55</v>
+      </c>
+      <c r="E7" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>94</v>
+      </c>
+      <c r="B8" t="n">
+        <v>28</v>
+      </c>
+      <c r="D8" t="n">
+        <v>57</v>
+      </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>80</v>
+      </c>
+      <c r="B9" t="n">
+        <v>92</v>
+      </c>
+      <c r="D9" t="n">
+        <v>18</v>
+      </c>
+      <c r="E9" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>98</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>65</v>
+      </c>
+      <c r="B11" t="n">
+        <v>33</v>
+      </c>
+      <c r="D11" t="n">
+        <v>78</v>
+      </c>
+      <c r="E11" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>35</v>
+      </c>
+      <c r="B12" t="n">
+        <v>46</v>
+      </c>
+      <c r="D12" t="n">
+        <v>13</v>
+      </c>
+      <c r="E12" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="n">
+        <v>44</v>
+      </c>
+      <c r="D13" t="n">
+        <v>85</v>
+      </c>
+      <c r="E13" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>89</v>
+      </c>
+      <c r="B14" t="n">
+        <v>96</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>68</v>
+      </c>
+      <c r="E15" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>43</v>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>74</v>
+      </c>
+      <c r="B17" t="n">
+        <v>87</v>
+      </c>
+      <c r="D17" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>71</v>
+      </c>
+      <c r="B18" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>51</v>
+      </c>
+      <c r="B19" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>25</v>
+      </c>
+      <c r="B20" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>84</v>
+      </c>
+      <c r="B21" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>9</v>
+      </c>
+      <c r="B22" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>58</v>
+      </c>
+      <c r="B23" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>47</v>
+      </c>
+      <c r="B24" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>82</v>
+      </c>
+      <c r="B25" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>99</v>
+      </c>
+      <c r="B26" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>21</v>
+      </c>
+      <c r="B27" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -3430,4 +3814,1590 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>84</v>
+      </c>
+      <c r="D2" t="n">
+        <v>61</v>
+      </c>
+      <c r="E2" t="n">
+        <v>38</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>65</v>
+      </c>
+      <c r="B3" t="n">
+        <v>59</v>
+      </c>
+      <c r="C3" t="n">
+        <v>63</v>
+      </c>
+      <c r="D3" t="n">
+        <v>36</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>78</v>
+      </c>
+      <c r="B4" t="n">
+        <v>53</v>
+      </c>
+      <c r="C4" t="n">
+        <v>51</v>
+      </c>
+      <c r="D4" t="n">
+        <v>72</v>
+      </c>
+      <c r="E4" t="n">
+        <v>62</v>
+      </c>
+      <c r="F4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>92</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>95</v>
+      </c>
+      <c r="D5" t="n">
+        <v>40</v>
+      </c>
+      <c r="E5" t="n">
+        <v>76</v>
+      </c>
+      <c r="F5" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" t="n">
+        <v>79</v>
+      </c>
+      <c r="C6" t="n">
+        <v>83</v>
+      </c>
+      <c r="D6" t="n">
+        <v>93</v>
+      </c>
+      <c r="E6" t="n">
+        <v>11</v>
+      </c>
+      <c r="F6" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>58</v>
+      </c>
+      <c r="B7" t="n">
+        <v>44</v>
+      </c>
+      <c r="C7" t="n">
+        <v>50</v>
+      </c>
+      <c r="D7" t="n">
+        <v>48</v>
+      </c>
+      <c r="E7" t="n">
+        <v>49</v>
+      </c>
+      <c r="F7" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>81</v>
+      </c>
+      <c r="B8" t="n">
+        <v>45</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" t="n">
+        <v>85</v>
+      </c>
+      <c r="F8" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>26</v>
+      </c>
+      <c r="B9" t="n">
+        <v>41</v>
+      </c>
+      <c r="C9" t="n">
+        <v>28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>37</v>
+      </c>
+      <c r="C10" t="n">
+        <v>64</v>
+      </c>
+      <c r="E10" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>46</v>
+      </c>
+      <c r="C11" t="n">
+        <v>94</v>
+      </c>
+      <c r="E11" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>67</v>
+      </c>
+      <c r="C12" t="n">
+        <v>47</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>15</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>31</v>
+      </c>
+      <c r="C14" t="n">
+        <v>32</v>
+      </c>
+      <c r="E14" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>68</v>
+      </c>
+      <c r="C15" t="n">
+        <v>42</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>34</v>
+      </c>
+      <c r="C16" t="n">
+        <v>73</v>
+      </c>
+      <c r="E16" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="E18" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>81</v>
+      </c>
+      <c r="B2" t="n">
+        <v>86</v>
+      </c>
+      <c r="C2" t="n">
+        <v>79</v>
+      </c>
+      <c r="E2" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" t="n">
+        <v>99</v>
+      </c>
+      <c r="C3" t="n">
+        <v>78</v>
+      </c>
+      <c r="E3" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>31</v>
+      </c>
+      <c r="B4" t="n">
+        <v>29</v>
+      </c>
+      <c r="C4" t="n">
+        <v>62</v>
+      </c>
+      <c r="E4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>40</v>
+      </c>
+      <c r="B5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B6" t="n">
+        <v>66</v>
+      </c>
+      <c r="C6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" t="n">
+        <v>77</v>
+      </c>
+      <c r="C7" t="n">
+        <v>91</v>
+      </c>
+      <c r="E7" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>11</v>
+      </c>
+      <c r="B8" t="n">
+        <v>37</v>
+      </c>
+      <c r="C8" t="n">
+        <v>84</v>
+      </c>
+      <c r="E8" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>70</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>89</v>
+      </c>
+      <c r="E9" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" t="n">
+        <v>44</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>96</v>
+      </c>
+      <c r="B11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C11" t="n">
+        <v>33</v>
+      </c>
+      <c r="E11" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>19</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>63</v>
+      </c>
+      <c r="E12" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>100</v>
+      </c>
+      <c r="C13" t="n">
+        <v>73</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>58</v>
+      </c>
+      <c r="B14" t="n">
+        <v>64</v>
+      </c>
+      <c r="C14" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>90</v>
+      </c>
+      <c r="B15" t="n">
+        <v>95</v>
+      </c>
+      <c r="C15" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>36</v>
+      </c>
+      <c r="B16" t="n">
+        <v>53</v>
+      </c>
+      <c r="C16" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>98</v>
+      </c>
+      <c r="B17" t="n">
+        <v>69</v>
+      </c>
+      <c r="C17" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>46</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>82</v>
+      </c>
+      <c r="B19" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>67</v>
+      </c>
+      <c r="B20" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>59</v>
+      </c>
+      <c r="B21" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+      <c r="B22" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>24</v>
+      </c>
+      <c r="B23" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>87</v>
+      </c>
+      <c r="B24" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>83</v>
+      </c>
+      <c r="F2" t="n">
+        <v>77</v>
+      </c>
+      <c r="G2" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>47</v>
+      </c>
+      <c r="C3" t="n">
+        <v>93</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" t="n">
+        <v>32</v>
+      </c>
+      <c r="G3" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>36</v>
+      </c>
+      <c r="C4" t="n">
+        <v>56</v>
+      </c>
+      <c r="D4" t="n">
+        <v>33</v>
+      </c>
+      <c r="E4" t="n">
+        <v>87</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>85</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" t="n">
+        <v>68</v>
+      </c>
+      <c r="E5" t="n">
+        <v>28</v>
+      </c>
+      <c r="F5" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>73</v>
+      </c>
+      <c r="C6" t="n">
+        <v>65</v>
+      </c>
+      <c r="D6" t="n">
+        <v>94</v>
+      </c>
+      <c r="E6" t="n">
+        <v>63</v>
+      </c>
+      <c r="F6" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>61</v>
+      </c>
+      <c r="C7" t="n">
+        <v>26</v>
+      </c>
+      <c r="D7" t="n">
+        <v>98</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>34</v>
+      </c>
+      <c r="C8" t="n">
+        <v>49</v>
+      </c>
+      <c r="D8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>90</v>
+      </c>
+      <c r="D9" t="n">
+        <v>29</v>
+      </c>
+      <c r="E9" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>80</v>
+      </c>
+      <c r="C10" t="n">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>89</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>18</v>
+      </c>
+      <c r="C12" t="n">
+        <v>9</v>
+      </c>
+      <c r="E12" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>30</v>
+      </c>
+      <c r="C13" t="n">
+        <v>42</v>
+      </c>
+      <c r="E13" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>92</v>
+      </c>
+      <c r="C14" t="n">
+        <v>35</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>95</v>
+      </c>
+      <c r="C15" t="n">
+        <v>79</v>
+      </c>
+      <c r="E15" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="n">
+        <v>96</v>
+      </c>
+      <c r="E16" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>76</v>
+      </c>
+      <c r="C17" t="n">
+        <v>91</v>
+      </c>
+      <c r="E17" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>58</v>
+      </c>
+      <c r="C18" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>40</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>43</v>
+      </c>
+      <c r="C22" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>27</v>
+      </c>
+      <c r="C23" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>44</v>
+      </c>
+      <c r="C24" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>82</v>
+      </c>
+      <c r="C25" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>39</v>
+      </c>
+      <c r="C26" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>48</v>
+      </c>
+      <c r="C28" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>66</v>
+      </c>
+      <c r="C29" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>84</v>
+      </c>
+      <c r="C30" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>47</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>56</v>
+      </c>
+      <c r="D2" t="n">
+        <v>26</v>
+      </c>
+      <c r="E2" t="n">
+        <v>80</v>
+      </c>
+      <c r="F2" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>31</v>
+      </c>
+      <c r="E3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F3" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>73</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>49</v>
+      </c>
+      <c r="E4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>75</v>
+      </c>
+      <c r="C5" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" t="n">
+        <v>14</v>
+      </c>
+      <c r="E5" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>13</v>
+      </c>
+      <c r="C6" t="n">
+        <v>67</v>
+      </c>
+      <c r="D6" t="n">
+        <v>98</v>
+      </c>
+      <c r="E6" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>41</v>
+      </c>
+      <c r="C7" t="n">
+        <v>63</v>
+      </c>
+      <c r="D7" t="n">
+        <v>45</v>
+      </c>
+      <c r="E7" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>39</v>
+      </c>
+      <c r="C8" t="n">
+        <v>99</v>
+      </c>
+      <c r="D8" t="n">
+        <v>18</v>
+      </c>
+      <c r="E8" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>53</v>
+      </c>
+      <c r="C9" t="n">
+        <v>84</v>
+      </c>
+      <c r="D9" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>54</v>
+      </c>
+      <c r="D10" t="n">
+        <v>23</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>91</v>
+      </c>
+      <c r="C11" t="n">
+        <v>58</v>
+      </c>
+      <c r="E11" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>27</v>
+      </c>
+      <c r="C12" t="n">
+        <v>34</v>
+      </c>
+      <c r="E12" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>21</v>
+      </c>
+      <c r="C13" t="n">
+        <v>35</v>
+      </c>
+      <c r="E13" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>30</v>
+      </c>
+      <c r="C14" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>19</v>
+      </c>
+      <c r="C15" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>36</v>
+      </c>
+      <c r="C16" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>83</v>
+      </c>
+      <c r="C17" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>71</v>
+      </c>
+      <c r="C18" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>81</v>
+      </c>
+      <c r="C19" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>100</v>
+      </c>
+      <c r="C20" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>24</v>
+      </c>
+      <c r="C21" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>92</v>
+      </c>
+      <c r="C23" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>59</v>
+      </c>
+      <c r="C24" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>87</v>
+      </c>
+      <c r="C25" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>50</v>
+      </c>
+      <c r="C26" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>86</v>
+      </c>
+      <c r="C27" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>55</v>
+      </c>
+      <c r="C28" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>96</v>
+      </c>
+      <c r="C29" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>61</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>65</v>
+      </c>
+      <c r="C31" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   Mentor_2.py 	modified:   __pycache__/Mentor_2.cpython-310.pyc 	modified:   nodes_inf.xlsx
</commit_message>
<xml_diff>
--- a/nodes_inf.xlsx
+++ b/nodes_inf.xlsx
@@ -75,6 +75,13 @@
     <sheet name="Backbones64" sheetId="66" state="visible" r:id="rId66"/>
     <sheet name="Backbones65" sheetId="67" state="visible" r:id="rId67"/>
     <sheet name="Backbones66" sheetId="68" state="visible" r:id="rId68"/>
+    <sheet name="Backbones67" sheetId="69" state="visible" r:id="rId69"/>
+    <sheet name="Backbones68" sheetId="70" state="visible" r:id="rId70"/>
+    <sheet name="Backbones69" sheetId="71" state="visible" r:id="rId71"/>
+    <sheet name="Backbones70" sheetId="72" state="visible" r:id="rId72"/>
+    <sheet name="Backbones71" sheetId="73" state="visible" r:id="rId73"/>
+    <sheet name="Backbones72" sheetId="74" state="visible" r:id="rId74"/>
+    <sheet name="Backbones73" sheetId="75" state="visible" r:id="rId75"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26943,6 +26950,377 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>78</v>
+      </c>
+      <c r="B2" t="n">
+        <v>51</v>
+      </c>
+      <c r="C2" t="n">
+        <v>31</v>
+      </c>
+      <c r="D2" t="n">
+        <v>33</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>66</v>
+      </c>
+      <c r="B3" t="n">
+        <v>46</v>
+      </c>
+      <c r="C3" t="n">
+        <v>28</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E3" t="n">
+        <v>35</v>
+      </c>
+      <c r="F3" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" t="n">
+        <v>76</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>94</v>
+      </c>
+      <c r="E4" t="n">
+        <v>91</v>
+      </c>
+      <c r="F4" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>85</v>
+      </c>
+      <c r="B5" t="n">
+        <v>90</v>
+      </c>
+      <c r="C5" t="n">
+        <v>52</v>
+      </c>
+      <c r="D5" t="n">
+        <v>43</v>
+      </c>
+      <c r="E5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F5" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>64</v>
+      </c>
+      <c r="D6" t="n">
+        <v>47</v>
+      </c>
+      <c r="E6" t="n">
+        <v>59</v>
+      </c>
+      <c r="F6" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B7" t="n">
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>54</v>
+      </c>
+      <c r="F7" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B8" t="n">
+        <v>34</v>
+      </c>
+      <c r="C8" t="n">
+        <v>73</v>
+      </c>
+      <c r="D8" t="n">
+        <v>41</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>65</v>
+      </c>
+      <c r="B9" t="n">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>98</v>
+      </c>
+      <c r="D9" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>86</v>
+      </c>
+      <c r="B10" t="n">
+        <v>99</v>
+      </c>
+      <c r="C10" t="n">
+        <v>40</v>
+      </c>
+      <c r="D10" t="n">
+        <v>82</v>
+      </c>
+      <c r="E10" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>96</v>
+      </c>
+      <c r="B11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C11" t="n">
+        <v>70</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>69</v>
+      </c>
+      <c r="B12" t="n">
+        <v>92</v>
+      </c>
+      <c r="C12" t="n">
+        <v>38</v>
+      </c>
+      <c r="E12" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>79</v>
+      </c>
+      <c r="B13" t="n">
+        <v>93</v>
+      </c>
+      <c r="C13" t="n">
+        <v>87</v>
+      </c>
+      <c r="E13" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>68</v>
+      </c>
+      <c r="B14" t="n">
+        <v>77</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>39</v>
+      </c>
+      <c r="B15" t="n">
+        <v>71</v>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>11</v>
+      </c>
+      <c r="B16" t="n">
+        <v>27</v>
+      </c>
+      <c r="C16" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>45</v>
+      </c>
+      <c r="B17" t="n">
+        <v>89</v>
+      </c>
+      <c r="C17" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>84</v>
+      </c>
+      <c r="B18" t="n">
+        <v>63</v>
+      </c>
+      <c r="C18" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>72</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>42</v>
+      </c>
+      <c r="B20" t="n">
+        <v>74</v>
+      </c>
+      <c r="C20" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>57</v>
+      </c>
+      <c r="C21" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>29</v>
+      </c>
+      <c r="C22" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>37</v>
+      </c>
+      <c r="C23" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="n">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -27343,6 +27721,2396 @@
     <row r="44">
       <c r="A44" t="n">
         <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>54</v>
+      </c>
+      <c r="B2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C2" t="n">
+        <v>87</v>
+      </c>
+      <c r="E2" t="n">
+        <v>48</v>
+      </c>
+      <c r="F2" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>57</v>
+      </c>
+      <c r="B3" t="n">
+        <v>26</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>74</v>
+      </c>
+      <c r="F3" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>13</v>
+      </c>
+      <c r="B4" t="n">
+        <v>94</v>
+      </c>
+      <c r="E4" t="n">
+        <v>92</v>
+      </c>
+      <c r="F4" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33</v>
+      </c>
+      <c r="B5" t="n">
+        <v>56</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>21</v>
+      </c>
+      <c r="F6" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>30</v>
+      </c>
+      <c r="B7" t="n">
+        <v>89</v>
+      </c>
+      <c r="E7" t="n">
+        <v>98</v>
+      </c>
+      <c r="F7" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>49</v>
+      </c>
+      <c r="B8" t="n">
+        <v>77</v>
+      </c>
+      <c r="F8" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>68</v>
+      </c>
+      <c r="B9" t="n">
+        <v>17</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>39</v>
+      </c>
+      <c r="B10" t="n">
+        <v>12</v>
+      </c>
+      <c r="F10" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>95</v>
+      </c>
+      <c r="B11" t="n">
+        <v>90</v>
+      </c>
+      <c r="F11" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>86</v>
+      </c>
+      <c r="B12" t="n">
+        <v>59</v>
+      </c>
+      <c r="F12" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>63</v>
+      </c>
+      <c r="B13" t="n">
+        <v>62</v>
+      </c>
+      <c r="F13" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" t="n">
+        <v>55</v>
+      </c>
+      <c r="F14" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>91</v>
+      </c>
+      <c r="B15" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>79</v>
+      </c>
+      <c r="B17" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>15</v>
+      </c>
+      <c r="B19" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>72</v>
+      </c>
+      <c r="B20" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>61</v>
+      </c>
+      <c r="B21" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>69</v>
+      </c>
+      <c r="B22" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32</v>
+      </c>
+      <c r="B23" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>99</v>
+      </c>
+      <c r="B24" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>6</v>
+      </c>
+      <c r="B25" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>53</v>
+      </c>
+      <c r="B26" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>96</v>
+      </c>
+      <c r="B27" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>80</v>
+      </c>
+      <c r="B28" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>16</v>
+      </c>
+      <c r="B29" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C2" t="n">
+        <v>28</v>
+      </c>
+      <c r="D2" t="n">
+        <v>82</v>
+      </c>
+      <c r="E2" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>46</v>
+      </c>
+      <c r="B3" t="n">
+        <v>94</v>
+      </c>
+      <c r="C3" t="n">
+        <v>65</v>
+      </c>
+      <c r="D3" t="n">
+        <v>87</v>
+      </c>
+      <c r="E3" t="n">
+        <v>31</v>
+      </c>
+      <c r="G3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>42</v>
+      </c>
+      <c r="B4" t="n">
+        <v>49</v>
+      </c>
+      <c r="C4" t="n">
+        <v>45</v>
+      </c>
+      <c r="E4" t="n">
+        <v>19</v>
+      </c>
+      <c r="G4" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>66</v>
+      </c>
+      <c r="B5" t="n">
+        <v>59</v>
+      </c>
+      <c r="C5" t="n">
+        <v>38</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="G5" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>55</v>
+      </c>
+      <c r="E6" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>95</v>
+      </c>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>99</v>
+      </c>
+      <c r="B8" t="n">
+        <v>75</v>
+      </c>
+      <c r="C8" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" t="n">
+        <v>93</v>
+      </c>
+      <c r="C9" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>71</v>
+      </c>
+      <c r="B10" t="n">
+        <v>85</v>
+      </c>
+      <c r="C10" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>56</v>
+      </c>
+      <c r="B11" t="n">
+        <v>68</v>
+      </c>
+      <c r="C11" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>80</v>
+      </c>
+      <c r="B12" t="n">
+        <v>98</v>
+      </c>
+      <c r="C12" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" t="n">
+        <v>72</v>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>48</v>
+      </c>
+      <c r="B14" t="n">
+        <v>40</v>
+      </c>
+      <c r="C14" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>29</v>
+      </c>
+      <c r="B15" t="n">
+        <v>50</v>
+      </c>
+      <c r="C15" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>53</v>
+      </c>
+      <c r="B16" t="n">
+        <v>77</v>
+      </c>
+      <c r="C16" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32</v>
+      </c>
+      <c r="B17" t="n">
+        <v>21</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="n">
+        <v>62</v>
+      </c>
+      <c r="C18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>33</v>
+      </c>
+      <c r="B19" t="n">
+        <v>14</v>
+      </c>
+      <c r="C19" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>96</v>
+      </c>
+      <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>70</v>
+      </c>
+      <c r="B21" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>83</v>
+      </c>
+      <c r="B22" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>81</v>
+      </c>
+      <c r="B23" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>64</v>
+      </c>
+      <c r="B24" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>69</v>
+      </c>
+      <c r="B25" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>41</v>
+      </c>
+      <c r="B26" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>86</v>
+      </c>
+      <c r="B27" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>34</v>
+      </c>
+      <c r="B28" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>73</v>
+      </c>
+      <c r="B2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>52</v>
+      </c>
+      <c r="B3" t="n">
+        <v>29</v>
+      </c>
+      <c r="C3" t="n">
+        <v>30</v>
+      </c>
+      <c r="E3" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>57</v>
+      </c>
+      <c r="B4" t="n">
+        <v>15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>26</v>
+      </c>
+      <c r="B5" t="n">
+        <v>37</v>
+      </c>
+      <c r="C5" t="n">
+        <v>49</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>100</v>
+      </c>
+      <c r="B6" t="n">
+        <v>31</v>
+      </c>
+      <c r="C6" t="n">
+        <v>72</v>
+      </c>
+      <c r="E6" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>23</v>
+      </c>
+      <c r="B7" t="n">
+        <v>32</v>
+      </c>
+      <c r="C7" t="n">
+        <v>94</v>
+      </c>
+      <c r="E7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>96</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>86</v>
+      </c>
+      <c r="B9" t="n">
+        <v>42</v>
+      </c>
+      <c r="C9" t="n">
+        <v>62</v>
+      </c>
+      <c r="E9" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>34</v>
+      </c>
+      <c r="B10" t="n">
+        <v>21</v>
+      </c>
+      <c r="C10" t="n">
+        <v>80</v>
+      </c>
+      <c r="E10" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>39</v>
+      </c>
+      <c r="B11" t="n">
+        <v>44</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>27</v>
+      </c>
+      <c r="C12" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>71</v>
+      </c>
+      <c r="B14" t="n">
+        <v>92</v>
+      </c>
+      <c r="C14" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>89</v>
+      </c>
+      <c r="B15" t="n">
+        <v>41</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>35</v>
+      </c>
+      <c r="B16" t="n">
+        <v>58</v>
+      </c>
+      <c r="C16" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>46</v>
+      </c>
+      <c r="B17" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>66</v>
+      </c>
+      <c r="B19" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>56</v>
+      </c>
+      <c r="B20" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>53</v>
+      </c>
+      <c r="B21" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>78</v>
+      </c>
+      <c r="B22" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>93</v>
+      </c>
+      <c r="B23" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>45</v>
+      </c>
+      <c r="B24" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>76</v>
+      </c>
+      <c r="B25" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>33</v>
+      </c>
+      <c r="B26" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>22</v>
+      </c>
+      <c r="B27" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>79</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>48</v>
+      </c>
+      <c r="B29" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>81</v>
+      </c>
+      <c r="B30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>74</v>
+      </c>
+      <c r="B31" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>75</v>
+      </c>
+      <c r="B32" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>84</v>
+      </c>
+      <c r="B33" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>47</v>
+      </c>
+      <c r="B34" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>38</v>
+      </c>
+      <c r="B2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D2" t="n">
+        <v>84</v>
+      </c>
+      <c r="E2" t="n">
+        <v>90</v>
+      </c>
+      <c r="F2" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>40</v>
+      </c>
+      <c r="B3" t="n">
+        <v>79</v>
+      </c>
+      <c r="C3" t="n">
+        <v>75</v>
+      </c>
+      <c r="D3" t="n">
+        <v>33</v>
+      </c>
+      <c r="E3" t="n">
+        <v>62</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>71</v>
+      </c>
+      <c r="B4" t="n">
+        <v>86</v>
+      </c>
+      <c r="C4" t="n">
+        <v>94</v>
+      </c>
+      <c r="D4" t="n">
+        <v>89</v>
+      </c>
+      <c r="E4" t="n">
+        <v>70</v>
+      </c>
+      <c r="F4" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>91</v>
+      </c>
+      <c r="B5" t="n">
+        <v>52</v>
+      </c>
+      <c r="C5" t="n">
+        <v>69</v>
+      </c>
+      <c r="D5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B6" t="n">
+        <v>98</v>
+      </c>
+      <c r="C6" t="n">
+        <v>26</v>
+      </c>
+      <c r="D6" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>48</v>
+      </c>
+      <c r="B7" t="n">
+        <v>57</v>
+      </c>
+      <c r="C7" t="n">
+        <v>44</v>
+      </c>
+      <c r="D7" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" t="n">
+        <v>63</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>72</v>
+      </c>
+      <c r="C9" t="n">
+        <v>56</v>
+      </c>
+      <c r="D9" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>64</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32</v>
+      </c>
+      <c r="D10" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>95</v>
+      </c>
+      <c r="C11" t="n">
+        <v>23</v>
+      </c>
+      <c r="D11" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>34</v>
+      </c>
+      <c r="D12" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>68</v>
+      </c>
+      <c r="D14" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>46</v>
+      </c>
+      <c r="D16" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>74</v>
+      </c>
+      <c r="D17" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="D18" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>59</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>39</v>
+      </c>
+      <c r="D21" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>82</v>
+      </c>
+      <c r="D22" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C2" t="n">
+        <v>74</v>
+      </c>
+      <c r="D2" t="n">
+        <v>14</v>
+      </c>
+      <c r="E2" t="n">
+        <v>43</v>
+      </c>
+      <c r="F2" t="n">
+        <v>18</v>
+      </c>
+      <c r="G2" t="n">
+        <v>83</v>
+      </c>
+      <c r="H2" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>67</v>
+      </c>
+      <c r="B3" t="n">
+        <v>41</v>
+      </c>
+      <c r="C3" t="n">
+        <v>99</v>
+      </c>
+      <c r="D3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F3" t="n">
+        <v>64</v>
+      </c>
+      <c r="G3" t="n">
+        <v>39</v>
+      </c>
+      <c r="H3" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>94</v>
+      </c>
+      <c r="B4" t="n">
+        <v>56</v>
+      </c>
+      <c r="C4" t="n">
+        <v>63</v>
+      </c>
+      <c r="D4" t="n">
+        <v>58</v>
+      </c>
+      <c r="E4" t="n">
+        <v>76</v>
+      </c>
+      <c r="F4" t="n">
+        <v>57</v>
+      </c>
+      <c r="G4" t="n">
+        <v>68</v>
+      </c>
+      <c r="H4" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>55</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>73</v>
+      </c>
+      <c r="F5" t="n">
+        <v>45</v>
+      </c>
+      <c r="G5" t="n">
+        <v>16</v>
+      </c>
+      <c r="H5" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>66</v>
+      </c>
+      <c r="B6" t="n">
+        <v>26</v>
+      </c>
+      <c r="C6" t="n">
+        <v>33</v>
+      </c>
+      <c r="D6" t="n">
+        <v>95</v>
+      </c>
+      <c r="E6" t="n">
+        <v>96</v>
+      </c>
+      <c r="F6" t="n">
+        <v>86</v>
+      </c>
+      <c r="H6" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>59</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>49</v>
+      </c>
+      <c r="F7" t="n">
+        <v>34</v>
+      </c>
+      <c r="H7" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>65</v>
+      </c>
+      <c r="E8" t="n">
+        <v>31</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>69</v>
+      </c>
+      <c r="D9" t="n">
+        <v>47</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>27</v>
+      </c>
+      <c r="D10" t="n">
+        <v>36</v>
+      </c>
+      <c r="E10" t="n">
+        <v>89</v>
+      </c>
+      <c r="F10" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" t="n">
+        <v>93</v>
+      </c>
+      <c r="E11" t="n">
+        <v>28</v>
+      </c>
+      <c r="F11" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>51</v>
+      </c>
+      <c r="D12" t="n">
+        <v>44</v>
+      </c>
+      <c r="E12" t="n">
+        <v>72</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>29</v>
+      </c>
+      <c r="D13" t="n">
+        <v>77</v>
+      </c>
+      <c r="E13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F13" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>20</v>
+      </c>
+      <c r="D14" t="n">
+        <v>48</v>
+      </c>
+      <c r="E14" t="n">
+        <v>54</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>75</v>
+      </c>
+      <c r="D15" t="n">
+        <v>62</v>
+      </c>
+      <c r="E15" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>38</v>
+      </c>
+      <c r="D16" t="n">
+        <v>53</v>
+      </c>
+      <c r="E16" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>35</v>
+      </c>
+      <c r="E17" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="E18" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>99</v>
+      </c>
+      <c r="B2" t="n">
+        <v>73</v>
+      </c>
+      <c r="C2" t="n">
+        <v>61</v>
+      </c>
+      <c r="D2" t="n">
+        <v>59</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F2" t="n">
+        <v>57</v>
+      </c>
+      <c r="G2" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>81</v>
+      </c>
+      <c r="B3" t="n">
+        <v>91</v>
+      </c>
+      <c r="D3" t="n">
+        <v>27</v>
+      </c>
+      <c r="E3" t="n">
+        <v>51</v>
+      </c>
+      <c r="F3" t="n">
+        <v>76</v>
+      </c>
+      <c r="G3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>62</v>
+      </c>
+      <c r="B4" t="n">
+        <v>70</v>
+      </c>
+      <c r="D4" t="n">
+        <v>45</v>
+      </c>
+      <c r="E4" t="n">
+        <v>94</v>
+      </c>
+      <c r="F4" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B5" t="n">
+        <v>46</v>
+      </c>
+      <c r="D5" t="n">
+        <v>22</v>
+      </c>
+      <c r="E5" t="n">
+        <v>89</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B6" t="n">
+        <v>92</v>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="n">
+        <v>32</v>
+      </c>
+      <c r="F6" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>36</v>
+      </c>
+      <c r="B7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="n">
+        <v>82</v>
+      </c>
+      <c r="F7" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>29</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>24</v>
+      </c>
+      <c r="F8" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>21</v>
+      </c>
+      <c r="B10" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>58</v>
+      </c>
+      <c r="B11" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>72</v>
+      </c>
+      <c r="B12" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>43</v>
+      </c>
+      <c r="B13" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>87</v>
+      </c>
+      <c r="B14" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>75</v>
+      </c>
+      <c r="B15" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>42</v>
+      </c>
+      <c r="B16" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>86</v>
+      </c>
+      <c r="B18" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>65</v>
+      </c>
+      <c r="B19" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>25</v>
+      </c>
+      <c r="B21" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>15</v>
+      </c>
+      <c r="B23" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>31</v>
+      </c>
+      <c r="B24" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   Main.py 	modified:   Mentor_2.py 	modified:   __pycache__/Mentor_2.cpython-310.pyc 	modified:   nodes_inf.xlsx
</commit_message>
<xml_diff>
--- a/nodes_inf.xlsx
+++ b/nodes_inf.xlsx
@@ -212,6 +212,14 @@
     <sheet name="Backbones201" sheetId="203" state="visible" r:id="rId203"/>
     <sheet name="Backbones202" sheetId="204" state="visible" r:id="rId204"/>
     <sheet name="Backbones203" sheetId="205" state="visible" r:id="rId205"/>
+    <sheet name="Backbones204" sheetId="206" state="visible" r:id="rId206"/>
+    <sheet name="Backbones205" sheetId="207" state="visible" r:id="rId207"/>
+    <sheet name="Backbones206" sheetId="208" state="visible" r:id="rId208"/>
+    <sheet name="Backbones207" sheetId="209" state="visible" r:id="rId209"/>
+    <sheet name="Backbones208" sheetId="210" state="visible" r:id="rId210"/>
+    <sheet name="Backbones209" sheetId="211" state="visible" r:id="rId211"/>
+    <sheet name="Backbones210" sheetId="212" state="visible" r:id="rId212"/>
+    <sheet name="Backbones211" sheetId="213" state="visible" r:id="rId213"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -48032,6 +48040,1548 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet206.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>67</v>
+      </c>
+      <c r="B2" t="n">
+        <v>32</v>
+      </c>
+      <c r="C2" t="n">
+        <v>65</v>
+      </c>
+      <c r="E2" t="n">
+        <v>62</v>
+      </c>
+      <c r="F2" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>43</v>
+      </c>
+      <c r="B3" t="n">
+        <v>95</v>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="E3" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>83</v>
+      </c>
+      <c r="B4" t="n">
+        <v>78</v>
+      </c>
+      <c r="C4" t="n">
+        <v>89</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>94</v>
+      </c>
+      <c r="B5" t="n">
+        <v>28</v>
+      </c>
+      <c r="C5" t="n">
+        <v>93</v>
+      </c>
+      <c r="E5" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C6" t="n">
+        <v>73</v>
+      </c>
+      <c r="E6" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>42</v>
+      </c>
+      <c r="B7" t="n">
+        <v>48</v>
+      </c>
+      <c r="C7" t="n">
+        <v>16</v>
+      </c>
+      <c r="E7" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>37</v>
+      </c>
+      <c r="B8" t="n">
+        <v>77</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>41</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>31</v>
+      </c>
+      <c r="E9" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>58</v>
+      </c>
+      <c r="B10" t="n">
+        <v>17</v>
+      </c>
+      <c r="C10" t="n">
+        <v>64</v>
+      </c>
+      <c r="E10" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>22</v>
+      </c>
+      <c r="B11" t="n">
+        <v>82</v>
+      </c>
+      <c r="C11" t="n">
+        <v>72</v>
+      </c>
+      <c r="E11" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>91</v>
+      </c>
+      <c r="B12" t="n">
+        <v>63</v>
+      </c>
+      <c r="C12" t="n">
+        <v>46</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>79</v>
+      </c>
+      <c r="B13" t="n">
+        <v>35</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15</v>
+      </c>
+      <c r="E13" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>49</v>
+      </c>
+      <c r="B14" t="n">
+        <v>85</v>
+      </c>
+      <c r="C14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>96</v>
+      </c>
+      <c r="B15" t="n">
+        <v>81</v>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>25</v>
+      </c>
+      <c r="B16" t="n">
+        <v>56</v>
+      </c>
+      <c r="C16" t="n">
+        <v>75</v>
+      </c>
+      <c r="E16" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>19</v>
+      </c>
+      <c r="B17" t="n">
+        <v>100</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>40</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>52</v>
+      </c>
+      <c r="B19" t="n">
+        <v>86</v>
+      </c>
+      <c r="C19" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>80</v>
+      </c>
+      <c r="B20" t="n">
+        <v>68</v>
+      </c>
+      <c r="C20" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>69</v>
+      </c>
+      <c r="C21" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>76</v>
+      </c>
+      <c r="C22" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>24</v>
+      </c>
+      <c r="C23" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>84</v>
+      </c>
+      <c r="C24" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>38</v>
+      </c>
+      <c r="C25" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>54</v>
+      </c>
+      <c r="C26" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>30</v>
+      </c>
+      <c r="C27" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>98</v>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>50</v>
+      </c>
+      <c r="C29" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet207.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>46</v>
+      </c>
+      <c r="B2" t="n">
+        <v>47</v>
+      </c>
+      <c r="C2" t="n">
+        <v>62</v>
+      </c>
+      <c r="D2" t="n">
+        <v>93</v>
+      </c>
+      <c r="E2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F2" t="n">
+        <v>67</v>
+      </c>
+      <c r="G2" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="n">
+        <v>80</v>
+      </c>
+      <c r="E3" t="n">
+        <v>81</v>
+      </c>
+      <c r="F3" t="n">
+        <v>56</v>
+      </c>
+      <c r="G3" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>57</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F4" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>38</v>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>82</v>
+      </c>
+      <c r="F5" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B6" t="n">
+        <v>68</v>
+      </c>
+      <c r="E6" t="n">
+        <v>84</v>
+      </c>
+      <c r="F6" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>52</v>
+      </c>
+      <c r="B7" t="n">
+        <v>23</v>
+      </c>
+      <c r="E7" t="n">
+        <v>92</v>
+      </c>
+      <c r="F7" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>22</v>
+      </c>
+      <c r="B8" t="n">
+        <v>26</v>
+      </c>
+      <c r="E8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" t="n">
+        <v>37</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>27</v>
+      </c>
+      <c r="B10" t="n">
+        <v>31</v>
+      </c>
+      <c r="E10" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>13</v>
+      </c>
+      <c r="B11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>24</v>
+      </c>
+      <c r="B12" t="n">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" t="n">
+        <v>79</v>
+      </c>
+      <c r="E13" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>86</v>
+      </c>
+      <c r="B14" t="n">
+        <v>71</v>
+      </c>
+      <c r="E14" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>49</v>
+      </c>
+      <c r="E15" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>19</v>
+      </c>
+      <c r="B16" t="n">
+        <v>30</v>
+      </c>
+      <c r="E16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>33</v>
+      </c>
+      <c r="B17" t="n">
+        <v>90</v>
+      </c>
+      <c r="E17" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>53</v>
+      </c>
+      <c r="B18" t="n">
+        <v>42</v>
+      </c>
+      <c r="E18" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>44</v>
+      </c>
+      <c r="B19" t="n">
+        <v>77</v>
+      </c>
+      <c r="E19" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>99</v>
+      </c>
+      <c r="B20" t="n">
+        <v>70</v>
+      </c>
+      <c r="E20" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>36</v>
+      </c>
+      <c r="B21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>89</v>
+      </c>
+      <c r="B22" t="n">
+        <v>41</v>
+      </c>
+      <c r="E22" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>20</v>
+      </c>
+      <c r="B24" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>28</v>
+      </c>
+      <c r="B25" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>91</v>
+      </c>
+      <c r="B26" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>76</v>
+      </c>
+      <c r="B27" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>43</v>
+      </c>
+      <c r="B28" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet208.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C2" t="n">
+        <v>40</v>
+      </c>
+      <c r="D2" t="n">
+        <v>39</v>
+      </c>
+      <c r="E2" t="n">
+        <v>85</v>
+      </c>
+      <c r="F2" t="n">
+        <v>36</v>
+      </c>
+      <c r="G2" t="n">
+        <v>75</v>
+      </c>
+      <c r="H2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>44</v>
+      </c>
+      <c r="B3" t="n">
+        <v>91</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22</v>
+      </c>
+      <c r="F3" t="n">
+        <v>98</v>
+      </c>
+      <c r="G3" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>35</v>
+      </c>
+      <c r="B4" t="n">
+        <v>68</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>58</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>71</v>
+      </c>
+      <c r="B5" t="n">
+        <v>52</v>
+      </c>
+      <c r="C5" t="n">
+        <v>99</v>
+      </c>
+      <c r="E5" t="n">
+        <v>70</v>
+      </c>
+      <c r="F5" t="n">
+        <v>55</v>
+      </c>
+      <c r="G5" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>79</v>
+      </c>
+      <c r="B6" t="n">
+        <v>19</v>
+      </c>
+      <c r="C6" t="n">
+        <v>87</v>
+      </c>
+      <c r="E6" t="n">
+        <v>67</v>
+      </c>
+      <c r="F6" t="n">
+        <v>26</v>
+      </c>
+      <c r="G6" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32</v>
+      </c>
+      <c r="C7" t="n">
+        <v>73</v>
+      </c>
+      <c r="E7" t="n">
+        <v>46</v>
+      </c>
+      <c r="F7" t="n">
+        <v>28</v>
+      </c>
+      <c r="G7" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>23</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+      <c r="E8" t="n">
+        <v>43</v>
+      </c>
+      <c r="G8" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>16</v>
+      </c>
+      <c r="C9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E9" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>27</v>
+      </c>
+      <c r="C10" t="n">
+        <v>31</v>
+      </c>
+      <c r="E10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>38</v>
+      </c>
+      <c r="C11" t="n">
+        <v>65</v>
+      </c>
+      <c r="E11" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>49</v>
+      </c>
+      <c r="C12" t="n">
+        <v>53</v>
+      </c>
+      <c r="E12" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>47</v>
+      </c>
+      <c r="C13" t="n">
+        <v>64</v>
+      </c>
+      <c r="E13" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>94</v>
+      </c>
+      <c r="C14" t="n">
+        <v>48</v>
+      </c>
+      <c r="E14" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>56</v>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>74</v>
+      </c>
+      <c r="E16" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7</v>
+      </c>
+      <c r="E17" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="C18" t="n">
+        <v>12</v>
+      </c>
+      <c r="E18" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>61</v>
+      </c>
+      <c r="C19" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>42</v>
+      </c>
+      <c r="C20" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>95</v>
+      </c>
+      <c r="C21" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>93</v>
+      </c>
+      <c r="C22" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>37</v>
+      </c>
+      <c r="C23" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>59</v>
+      </c>
+      <c r="C24" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>66</v>
+      </c>
+      <c r="C25" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet209.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>61</v>
+      </c>
+      <c r="B2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" t="n">
+        <v>46</v>
+      </c>
+      <c r="D2" t="n">
+        <v>29</v>
+      </c>
+      <c r="E2" t="n">
+        <v>91</v>
+      </c>
+      <c r="F2" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>66</v>
+      </c>
+      <c r="B3" t="n">
+        <v>71</v>
+      </c>
+      <c r="C3" t="n">
+        <v>99</v>
+      </c>
+      <c r="D3" t="n">
+        <v>31</v>
+      </c>
+      <c r="E3" t="n">
+        <v>86</v>
+      </c>
+      <c r="F3" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>57</v>
+      </c>
+      <c r="B4" t="n">
+        <v>59</v>
+      </c>
+      <c r="C4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D4" t="n">
+        <v>52</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>38</v>
+      </c>
+      <c r="B5" t="n">
+        <v>56</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>23</v>
+      </c>
+      <c r="E5" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>55</v>
+      </c>
+      <c r="C6" t="n">
+        <v>28</v>
+      </c>
+      <c r="D6" t="n">
+        <v>42</v>
+      </c>
+      <c r="E6" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>78</v>
+      </c>
+      <c r="B7" t="n">
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>76</v>
+      </c>
+      <c r="D7" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>92</v>
+      </c>
+      <c r="B8" t="n">
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
+        <v>41</v>
+      </c>
+      <c r="D8" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>19</v>
+      </c>
+      <c r="C9" t="n">
+        <v>17</v>
+      </c>
+      <c r="D9" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>90</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
+        <v>48</v>
+      </c>
+      <c r="D11" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>49</v>
+      </c>
+      <c r="D12" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>63</v>
+      </c>
+      <c r="C13" t="n">
+        <v>69</v>
+      </c>
+      <c r="D13" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>81</v>
+      </c>
+      <c r="C14" t="n">
+        <v>30</v>
+      </c>
+      <c r="D14" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32</v>
+      </c>
+      <c r="C15" t="n">
+        <v>82</v>
+      </c>
+      <c r="D15" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>37</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>80</v>
+      </c>
+      <c r="C17" t="n">
+        <v>96</v>
+      </c>
+      <c r="D17" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>64</v>
+      </c>
+      <c r="C18" t="n">
+        <v>33</v>
+      </c>
+      <c r="D18" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>43</v>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>7</v>
+      </c>
+      <c r="C20" t="n">
+        <v>68</v>
+      </c>
+      <c r="D20" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>16</v>
+      </c>
+      <c r="C21" t="n">
+        <v>39</v>
+      </c>
+      <c r="D21" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>62</v>
+      </c>
+      <c r="C22" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>72</v>
+      </c>
+      <c r="C23" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -48410,6 +49960,1632 @@
     <row r="33">
       <c r="A33" t="n">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet210.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>65</v>
+      </c>
+      <c r="B2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E2" t="n">
+        <v>43</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B3" t="n">
+        <v>86</v>
+      </c>
+      <c r="C3" t="n">
+        <v>38</v>
+      </c>
+      <c r="D3" t="n">
+        <v>51</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>80</v>
+      </c>
+      <c r="B4" t="n">
+        <v>95</v>
+      </c>
+      <c r="C4" t="n">
+        <v>57</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>16</v>
+      </c>
+      <c r="G4" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B5" t="n">
+        <v>42</v>
+      </c>
+      <c r="C5" t="n">
+        <v>79</v>
+      </c>
+      <c r="D5" t="n">
+        <v>78</v>
+      </c>
+      <c r="E5" t="n">
+        <v>45</v>
+      </c>
+      <c r="G5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>87</v>
+      </c>
+      <c r="B6" t="n">
+        <v>98</v>
+      </c>
+      <c r="C6" t="n">
+        <v>74</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="n">
+        <v>96</v>
+      </c>
+      <c r="C7" t="n">
+        <v>23</v>
+      </c>
+      <c r="E7" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>94</v>
+      </c>
+      <c r="B8" t="n">
+        <v>73</v>
+      </c>
+      <c r="C8" t="n">
+        <v>58</v>
+      </c>
+      <c r="E8" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" t="n">
+        <v>67</v>
+      </c>
+      <c r="C10" t="n">
+        <v>56</v>
+      </c>
+      <c r="E10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33</v>
+      </c>
+      <c r="C11" t="n">
+        <v>81</v>
+      </c>
+      <c r="E11" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>85</v>
+      </c>
+      <c r="C12" t="n">
+        <v>91</v>
+      </c>
+      <c r="E12" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>44</v>
+      </c>
+      <c r="C13" t="n">
+        <v>47</v>
+      </c>
+      <c r="E13" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>22</v>
+      </c>
+      <c r="C14" t="n">
+        <v>93</v>
+      </c>
+      <c r="E14" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>66</v>
+      </c>
+      <c r="C15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>37</v>
+      </c>
+      <c r="C16" t="n">
+        <v>17</v>
+      </c>
+      <c r="E16" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="C17" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>63</v>
+      </c>
+      <c r="C18" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>82</v>
+      </c>
+      <c r="C19" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>54</v>
+      </c>
+      <c r="C20" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>62</v>
+      </c>
+      <c r="C21" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>31</v>
+      </c>
+      <c r="C22" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>46</v>
+      </c>
+      <c r="C23" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet211.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>87</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>71</v>
+      </c>
+      <c r="E2" t="n">
+        <v>61</v>
+      </c>
+      <c r="F2" t="n">
+        <v>67</v>
+      </c>
+      <c r="G2" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>55</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" t="n">
+        <v>79</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>53</v>
+      </c>
+      <c r="C4" t="n">
+        <v>70</v>
+      </c>
+      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" t="n">
+        <v>46</v>
+      </c>
+      <c r="F4" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>58</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
+        <v>42</v>
+      </c>
+      <c r="F5" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>76</v>
+      </c>
+      <c r="C6" t="n">
+        <v>68</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" t="n">
+        <v>62</v>
+      </c>
+      <c r="F6" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>30</v>
+      </c>
+      <c r="C7" t="n">
+        <v>43</v>
+      </c>
+      <c r="E7" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>40</v>
+      </c>
+      <c r="C8" t="n">
+        <v>83</v>
+      </c>
+      <c r="E8" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>82</v>
+      </c>
+      <c r="C9" t="n">
+        <v>96</v>
+      </c>
+      <c r="E9" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>65</v>
+      </c>
+      <c r="C10" t="n">
+        <v>91</v>
+      </c>
+      <c r="E10" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>36</v>
+      </c>
+      <c r="C11" t="n">
+        <v>69</v>
+      </c>
+      <c r="E11" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" t="n">
+        <v>51</v>
+      </c>
+      <c r="E12" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>59</v>
+      </c>
+      <c r="C13" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>90</v>
+      </c>
+      <c r="C14" t="n">
+        <v>73</v>
+      </c>
+      <c r="E14" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="C15" t="n">
+        <v>99</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>38</v>
+      </c>
+      <c r="C16" t="n">
+        <v>13</v>
+      </c>
+      <c r="E16" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>47</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>57</v>
+      </c>
+      <c r="C18" t="n">
+        <v>21</v>
+      </c>
+      <c r="E18" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>41</v>
+      </c>
+      <c r="C19" t="n">
+        <v>78</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>23</v>
+      </c>
+      <c r="C20" t="n">
+        <v>52</v>
+      </c>
+      <c r="E20" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>49</v>
+      </c>
+      <c r="C21" t="n">
+        <v>33</v>
+      </c>
+      <c r="E21" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>44</v>
+      </c>
+      <c r="C22" t="n">
+        <v>84</v>
+      </c>
+      <c r="E22" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>63</v>
+      </c>
+      <c r="C23" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>45</v>
+      </c>
+      <c r="C24" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>54</v>
+      </c>
+      <c r="C25" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>64</v>
+      </c>
+      <c r="C26" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet212.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n">
+        <v>95</v>
+      </c>
+      <c r="C2" t="n">
+        <v>93</v>
+      </c>
+      <c r="D2" t="n">
+        <v>49</v>
+      </c>
+      <c r="E2" t="n">
+        <v>90</v>
+      </c>
+      <c r="F2" t="n">
+        <v>31</v>
+      </c>
+      <c r="G2" t="n">
+        <v>75</v>
+      </c>
+      <c r="H2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>91</v>
+      </c>
+      <c r="B3" t="n">
+        <v>55</v>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>72</v>
+      </c>
+      <c r="E3" t="n">
+        <v>17</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>62</v>
+      </c>
+      <c r="B4" t="n">
+        <v>96</v>
+      </c>
+      <c r="C4" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" t="n">
+        <v>46</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>86</v>
+      </c>
+      <c r="G4" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B5" t="n">
+        <v>44</v>
+      </c>
+      <c r="C5" t="n">
+        <v>26</v>
+      </c>
+      <c r="E5" t="n">
+        <v>52</v>
+      </c>
+      <c r="F5" t="n">
+        <v>53</v>
+      </c>
+      <c r="G5" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>78</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+      <c r="E6" t="n">
+        <v>76</v>
+      </c>
+      <c r="F6" t="n">
+        <v>59</v>
+      </c>
+      <c r="G6" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>89</v>
+      </c>
+      <c r="C7" t="n">
+        <v>68</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>79</v>
+      </c>
+      <c r="C8" t="n">
+        <v>77</v>
+      </c>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>23</v>
+      </c>
+      <c r="C9" t="n">
+        <v>69</v>
+      </c>
+      <c r="E9" t="n">
+        <v>43</v>
+      </c>
+      <c r="F9" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>84</v>
+      </c>
+      <c r="C10" t="n">
+        <v>92</v>
+      </c>
+      <c r="E10" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>83</v>
+      </c>
+      <c r="C11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>16</v>
+      </c>
+      <c r="E12" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet213.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" t="n">
+        <v>32</v>
+      </c>
+      <c r="C2" t="n">
+        <v>78</v>
+      </c>
+      <c r="E2" t="n">
+        <v>42</v>
+      </c>
+      <c r="F2" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2" t="n">
+        <v>89</v>
+      </c>
+      <c r="H2" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>59</v>
+      </c>
+      <c r="B3" t="n">
+        <v>46</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>52</v>
+      </c>
+      <c r="G3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>82</v>
+      </c>
+      <c r="B4" t="n">
+        <v>15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>23</v>
+      </c>
+      <c r="E4" t="n">
+        <v>40</v>
+      </c>
+      <c r="F4" t="n">
+        <v>73</v>
+      </c>
+      <c r="G4" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>56</v>
+      </c>
+      <c r="B5" t="n">
+        <v>49</v>
+      </c>
+      <c r="C5" t="n">
+        <v>34</v>
+      </c>
+      <c r="E5" t="n">
+        <v>61</v>
+      </c>
+      <c r="F5" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" t="n">
+        <v>63</v>
+      </c>
+      <c r="C6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>47</v>
+      </c>
+      <c r="F6" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>98</v>
+      </c>
+      <c r="B7" t="n">
+        <v>75</v>
+      </c>
+      <c r="C7" t="n">
+        <v>69</v>
+      </c>
+      <c r="E7" t="n">
+        <v>58</v>
+      </c>
+      <c r="F7" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>93</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>33</v>
+      </c>
+      <c r="F8" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>77</v>
+      </c>
+      <c r="B9" t="n">
+        <v>21</v>
+      </c>
+      <c r="F9" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>16</v>
+      </c>
+      <c r="B10" t="n">
+        <v>24</v>
+      </c>
+      <c r="F10" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" t="n">
+        <v>22</v>
+      </c>
+      <c r="F11" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>92</v>
+      </c>
+      <c r="B13" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>35</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>25</v>
+      </c>
+      <c r="B16" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>53</v>
+      </c>
+      <c r="B17" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>